<commit_message>
Add calls to `PATH_TO_CREDENTIALS_FILE`
</commit_message>
<xml_diff>
--- a/docs/source/function_call_chain_connections.xlsx
+++ b/docs/source/function_call_chain_connections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereiskind\nolcat\docs\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE236DCA-53A8-4E67-8CC6-305EB794FD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4E8902-CB9D-4B9D-8E2B-04331D0AE408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{44512B9D-2A90-4646-8933-428A99F14C9B}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="464">
   <si>
     <t>Calling Function</t>
   </si>
@@ -1438,7 +1438,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1450,6 +1450,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1475,19 +1482,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1514,6 +1518,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF9C0006"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1526,11 +1535,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A35B55CA-3D7A-4630-80A4-302CC6486C4B}" name="Table3" displayName="Table3" ref="A1:C385" totalsRowShown="0">
-  <autoFilter ref="A1:C385" xr:uid="{A35B55CA-3D7A-4630-80A4-302CC6486C4B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A35B55CA-3D7A-4630-80A4-302CC6486C4B}" name="Table3" displayName="Table3" ref="A1:C387" totalsRowShown="0">
+  <autoFilter ref="A1:C387" xr:uid="{A35B55CA-3D7A-4630-80A4-302CC6486C4B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7FD1105F-C7A5-4E16-926A-A61CDD080060}" name="Called Node Name"/>
-    <tableColumn id="2" xr3:uid="{CE4DE19D-EA52-4CF0-9B0C-C1DFDE7DD080}" name="Called Function" dataDxfId="3">
+    <tableColumn id="2" xr3:uid="{CE4DE19D-EA52-4CF0-9B0C-C1DFDE7DD080}" name="Called Function" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{C2024EA6-7D5C-4C8B-9CCD-AF563856B1E1}" name="Calling Function"/>
@@ -1540,13 +1549,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{71A6869D-4B7A-4FAA-A02E-10A2F1466D47}" name="Table2" displayName="Table2" ref="A1:D385" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{71A6869D-4B7A-4FAA-A02E-10A2F1466D47}" name="Table2" displayName="Table2" ref="A1:D385" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:D385" xr:uid="{A6211418-BCE9-480F-9AC5-9CD507C26481}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{69CD15C3-5B02-4859-BD05-680C3DBFC908}" name="Node Name"/>
     <tableColumn id="2" xr3:uid="{3B8ECDB6-A578-4E02-AC3C-7452D338C2BE}" name="Function Name"/>
     <tableColumn id="3" xr3:uid="{D3E5C4D2-15D2-41F6-B02F-14A3A95B3654}" name="Cluster"/>
-    <tableColumn id="4" xr3:uid="{C97D9CDF-DBD9-426B-97D0-179A8305BFF1}" name="Order Within Cluster" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C97D9CDF-DBD9-426B-97D0-179A8305BFF1}" name="Order Within Cluster" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1869,10 +1878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202E7D9A-A4E5-4FC3-B37C-A36A5067E5D4}">
-  <dimension ref="A1:C385"/>
+  <dimension ref="A1:C387"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F1048576"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1901,3458 +1910,3482 @@
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
         <v>PATH_TO_CREDENTIALS_FILE</v>
       </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>calculate_depreciated_ACRL_60b</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>PATH_TO_CREDENTIALS_FILE</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>calculate_depreciated_ACRL_63</v>
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>PATH_TO_CREDENTIALS_FILE</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>calculate_ACRL_61a</v>
+        <v>calculate_depreciated_ACRL_60b</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>calculate_ACRL_61b</v>
+        <v>calculate_depreciated_ACRL_63</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>calculate_ARL_18</v>
+        <v>calculate_ACRL_61a</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>calculate_ARL_19</v>
+        <v>calculate_ACRL_61b</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>calculate_ARL_20</v>
+        <v>calculate_ARL_18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_usage_tracking_records_for_fiscal_year</v>
+        <v>calculate_ARL_19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>collect_fiscal_year_usage_statistics</v>
+        <v>calculate_ARL_20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B12" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>state_data_types</v>
+        <v>create_usage_tracking_records_for_fiscal_year</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>add_annual_statistic_value</v>
+        <v>collect_fiscal_year_usage_statistics</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="str">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
         <v>state_data_types</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B15" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>get_statisticsSources_records</v>
+        <v>add_annual_statistic_value</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>get_resourceSources_records</v>
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>state_data_types</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>add_note</v>
+        <v>get_statisticsSources_records</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B18" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>state_data_types</v>
+        <v>get_resourceSources_records</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>state_data_types</v>
+        <v>28</v>
+      </c>
+      <c r="B19" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>add_note</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>fetch_SUSHI_information</v>
+        <v>31</v>
+      </c>
+      <c r="B20" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>state_data_types</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>_harvest_R5_SUSHI</v>
+        <v>33</v>
+      </c>
+      <c r="B21" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>state_data_types</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B22" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>_harvest_single_report</v>
+        <v>fetch_SUSHI_information</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B23" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>_check_if_data_in_database</v>
+        <v>_harvest_R5_SUSHI</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B24" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>collect_usage_statistics</v>
+        <v>_harvest_single_report</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B25" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>add_note</v>
+        <v>_check_if_data_in_database</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B26" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>state_data_types</v>
+        <v>collect_usage_statistics</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>state_data_types</v>
+        <v>38</v>
+      </c>
+      <c r="B27" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>add_note</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>add_access_stop_date</v>
+        <v>40</v>
+      </c>
+      <c r="B28" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>state_data_types</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>remove_access_stop_date</v>
+        <v>42</v>
+      </c>
+      <c r="B29" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>state_data_types</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B30" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>change_StatisticsSource</v>
+        <v>add_access_stop_date</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B31" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>add_note</v>
+        <v>remove_access_stop_date</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B32" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>state_data_types</v>
+        <v>change_StatisticsSource</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B33" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>state_data_types</v>
+        <v>46</v>
+      </c>
+      <c r="B33" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>add_note</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" t="str">
+        <v>48</v>
+      </c>
+      <c r="B34" s="2" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
         <v>state_data_types</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>collect_annual_usage_statistics</v>
+        <v>50</v>
+      </c>
+      <c r="B35" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>state_data_types</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>upload_nonstandard_usage_file</v>
+        <v>52</v>
+      </c>
+      <c r="B36" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>state_data_types</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B37" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>download_nonstandard_usage_file</v>
+        <v>collect_annual_usage_statistics</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B38" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>state_data_types</v>
+        <v>upload_nonstandard_usage_file</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B39" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>make_SUSHI_call</v>
+        <v>download_nonstandard_usage_file</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>_make_API_call</v>
+        <v>57</v>
+      </c>
+      <c r="B40" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>state_data_types</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B41" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>_convert_Response_to_JSON</v>
+        <v>make_SUSHI_call</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B42" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>_save_raw_Response_text</v>
+        <v>_make_API_call</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B43" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>_handle_SUSHI_exceptions</v>
+        <v>_convert_Response_to_JSON</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B44" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>_evaluate_individual_SUSHI_exception</v>
+        <v>_save_raw_Response_text</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B45" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>_stdout_API_response_based_on_size</v>
+        <v>_handle_SUSHI_exceptions</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B46" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_dataframe</v>
+        <v>_evaluate_individual_SUSHI_exception</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B47" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_dataframe</v>
+        <v>_stdout_API_response_based_on_size</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>_transform_R5_JSON</v>
+        <v>67</v>
+      </c>
+      <c r="B48" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>create_dataframe</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>72</v>
-      </c>
-      <c r="B49" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>_transform_R5b1_JSON</v>
+        <v>70</v>
+      </c>
+      <c r="B49" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>create_dataframe</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B50" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>_serialize_dates</v>
+        <v>_transform_R5_JSON</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B51" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>annual_stats_homepage</v>
+        <v>_transform_R5b1_JSON</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B52" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>show_fiscal_year_details</v>
+        <v>_serialize_dates</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B53" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>ingest_usage_homepage</v>
+        <v>annual_stats_homepage</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B54" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>upload_COUNTER_data</v>
+        <v>show_fiscal_year_details</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B55" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>harvest_SUSHI_statistics</v>
+        <v>ingest_usage_homepage</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B56" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>upload_non_COUNTER_reports</v>
+        <v>upload_COUNTER_data</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B57" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>collect_FY_and_vendor_data</v>
+        <v>harvest_SUSHI_statistics</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B58" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>collect_sources_data</v>
+        <v>upload_non_COUNTER_reports</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B59" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>collect_AUCT_and_historical_COUNTER_data</v>
+        <v>collect_FY_and_vendor_data</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B60" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>upload_historical_non_COUNTER_usage</v>
+        <v>collect_sources_data</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B61" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>data_load_complete</v>
+        <v>collect_AUCT_and_historical_COUNTER_data</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B62" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>login_homepage</v>
+        <v>upload_historical_non_COUNTER_usage</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B63" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>view_lists_homepage</v>
+        <v>data_load_complete</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B64" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>view_list_record</v>
+        <v>login_homepage</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B65" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>edit_list_record</v>
+        <v>view_lists_homepage</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B66" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_COUNTER_fixed_vocab_list</v>
+        <v>view_list_record</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B67" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>set_encoding</v>
+        <v>edit_list_record</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B68" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_downloads_folder</v>
+        <v>create_COUNTER_fixed_vocab_list</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B69" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>view_usage_homepage</v>
+        <v>set_encoding</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B70" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>run_custom_SQL_query</v>
+        <v>create_downloads_folder</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B71" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>use_predefined_SQL_query</v>
+        <v>view_usage_homepage</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B72" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>start_query_wizard</v>
+        <v>run_custom_SQL_query</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B73" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>query_wizard_sort_redirect</v>
+        <v>use_predefined_SQL_query</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B74" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>construct_PR_query_with_wizard</v>
+        <v>start_query_wizard</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B75" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>construct_DR_query_with_wizard</v>
+        <v>query_wizard_sort_redirect</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B76" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>construct_TR_query_with_wizard</v>
+        <v>construct_PR_query_with_wizard</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B77" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>construct_IR_query_with_wizard</v>
+        <v>construct_DR_query_with_wizard</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B78" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>download_non_COUNTER_usage</v>
+        <v>construct_TR_query_with_wizard</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B79" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>filter_empty_parentheses</v>
+        <v>construct_IR_query_with_wizard</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B80" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>configure_logging</v>
+        <v>download_non_COUNTER_usage</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B81" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>page_not_found</v>
+        <v>filter_empty_parentheses</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B82" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>internal_server_error</v>
+        <v>configure_logging</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B83" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_app</v>
+        <v>page_not_found</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B84" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>"create_app.create_db"</v>
+        <v>internal_server_error</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B85" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>"create_app.homepage"</v>
+        <v>create_app</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B86" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>"create_app.download_file"</v>
+        <v>"create_app.create_db"</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B87" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>last_day_of_month</v>
+        <v>"create_app.homepage"</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B88" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>first_new_PK_value</v>
+        <v>"create_app.download_file"</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B89" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>return_string_of_dataframe_info</v>
+        <v>last_day_of_month</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B90" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>change_single_field_dataframe_into_series</v>
+        <v>first_new_PK_value</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B91" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>restore_boolean_values_to_boolean_field</v>
+        <v>return_string_of_dataframe_info</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B92" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>upload_file_to_S3_bucket</v>
+        <v>change_single_field_dataframe_into_series</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B93" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_AUCT_SelectField_options</v>
+        <v>restore_boolean_values_to_boolean_field</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B94" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>load_data_into_database</v>
+        <v>upload_file_to_S3_bucket</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B95" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>query_database</v>
+        <v>create_AUCT_SelectField_options</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B96" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>check_if_data_already_in_COUNTERData</v>
+        <v>load_data_into_database</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B97" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>truncate_longer_lines</v>
+        <v>query_database</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B98" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>update_database</v>
+        <v>check_if_data_already_in_COUNTERData</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B99" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>save_unconverted_data_via_upload</v>
+        <v>truncate_longer_lines</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B100" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>ISSN_regex</v>
+        <v>update_database</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B101" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>ISBN_regex</v>
+        <v>save_unconverted_data_via_upload</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B102" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>extract_value_from_single_value_df</v>
+        <v>ISSN_regex</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B103" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>AWS_timestamp_format</v>
+        <v>ISBN_regex</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B104" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>non_COUNTER_file_name_regex</v>
+        <v>extract_value_from_single_value_df</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B105" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>empty_string_regex</v>
+        <v>AWS_timestamp_format</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B106" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>file_extensions_and_mimetypes</v>
+        <v>non_COUNTER_file_name_regex</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B107" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>format_list_for_stdout</v>
+        <v>empty_string_regex</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B108" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>remove_IDE_spacing_from_statement</v>
+        <v>file_extensions_and_mimetypes</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B109" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>initialize_relation_class_object_statement</v>
+        <v>format_list_for_stdout</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B110" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>fixture_variable_value_declaration_statement</v>
+        <v>remove_IDE_spacing_from_statement</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B111" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>unable_to_convert_SUSHI_data_to_dataframe_statement</v>
+        <v>initialize_relation_class_object_statement</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B112" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>unable_to_get_updated_primary_key_values_statement</v>
+        <v>fixture_variable_value_declaration_statement</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B113" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>Flask_error_statement</v>
+        <v>unable_to_convert_SUSHI_data_to_dataframe_statement</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B114" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>file_IO_statement</v>
+        <v>unable_to_get_updated_primary_key_values_statement</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B115" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>list_folder_contents_statement</v>
+        <v>Flask_error_statement</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B116" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>check_if_file_exists_statement</v>
+        <v>file_IO_statement</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B117" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>failed_upload_to_S3_statement</v>
+        <v>list_folder_contents_statement</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B118" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>unable_to_delete_test_file_in_S3_statement</v>
+        <v>check_if_file_exists_statement</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B119" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>upload_file_to_S3_bucket_success_regex</v>
+        <v>failed_upload_to_S3_statement</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B120" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>upload_nonstandard_usage_file_success_regex</v>
+        <v>unable_to_delete_test_file_in_S3_statement</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B121" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>return_value_from_query_statement</v>
+        <v>upload_file_to_S3_bucket_success_regex</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B122" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>return_dataframe_from_query_statement</v>
+        <v>upload_nonstandard_usage_file_success_regex</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B123" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>database_query_fail_statement</v>
+        <v>return_value_from_query_statement</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B124" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>database_update_fail_statement</v>
+        <v>return_dataframe_from_query_statement</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B125" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>add_data_success_and_update_database_fail_statement</v>
+        <v>database_query_fail_statement</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B126" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>database_function_skip_statements</v>
+        <v>database_update_fail_statement</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B127" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>load_data_into_database_success_regex</v>
+        <v>add_data_success_and_update_database_fail_statement</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B128" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>update_database_success_regex</v>
+        <v>database_function_skip_statements</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B129" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>successful_SUSHI_call_statement</v>
+        <v>load_data_into_database_success_regex</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B130" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>harvest_R5_SUSHI_success_statement</v>
+        <v>update_database_success_regex</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B131" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>failed_SUSHI_call_statement</v>
+        <v>successful_SUSHI_call_statement</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B132" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>no_data_returned_by_SUSHI_statement</v>
+        <v>harvest_R5_SUSHI_success_statement</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B133" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>attempted_SUSHI_call_with_invalid_dates_statement</v>
+        <v>failed_SUSHI_call_statement</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B134" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>reports_with_no_usage_regex</v>
+        <v>no_data_returned_by_SUSHI_statement</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B135" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>skip_test_due_to_SUSHI_error_regex</v>
+        <v>attempted_SUSHI_call_with_invalid_dates_statement</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B136" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>fiscalYears_relation</v>
+        <v>reports_with_no_usage_regex</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B137" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>annualStatistics_relation</v>
+        <v>skip_test_due_to_SUSHI_error_regex</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>172</v>
-      </c>
-      <c r="B138" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendors_relation</v>
+        <v>168</v>
+      </c>
+      <c r="B138" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>fiscalYears_relation</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>173</v>
-      </c>
-      <c r="B139" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendorNotes_relation</v>
+        <v>170</v>
+      </c>
+      <c r="B139" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>annualStatistics_relation</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>174</v>
-      </c>
-      <c r="B140" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsSources_relation</v>
+        <v>172</v>
+      </c>
+      <c r="B140" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>vendors_relation</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>175</v>
-      </c>
-      <c r="B141" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsSourceNotes_relation</v>
+        <v>173</v>
+      </c>
+      <c r="B141" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>vendorNotes_relation</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>176</v>
-      </c>
-      <c r="B142" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>resourceSources_relation</v>
+        <v>174</v>
+      </c>
+      <c r="B142" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsSources_relation</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>177</v>
-      </c>
-      <c r="B143" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>resourceSourceNotes_relation</v>
+        <v>175</v>
+      </c>
+      <c r="B143" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsSourceNotes_relation</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>178</v>
-      </c>
-      <c r="B144" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsResourceSources_relation</v>
+        <v>176</v>
+      </c>
+      <c r="B144" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>resourceSources_relation</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>179</v>
-      </c>
-      <c r="B145" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>annualUsageCollectionTracking_relation</v>
+        <v>177</v>
+      </c>
+      <c r="B145" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>resourceSourceNotes_relation</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>180</v>
-      </c>
-      <c r="B146" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_0_2017_relation</v>
+        <v>178</v>
+      </c>
+      <c r="B146" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsResourceSources_relation</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>181</v>
-      </c>
-      <c r="B147" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_1_2017_relation</v>
+        <v>179</v>
+      </c>
+      <c r="B147" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>annualUsageCollectionTracking_relation</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>182</v>
-      </c>
-      <c r="B148" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_2_2017_relation</v>
+        <v>180</v>
+      </c>
+      <c r="B148" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_0_2017_relation</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>183</v>
-      </c>
-      <c r="B149" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_0_2018_relation</v>
+        <v>181</v>
+      </c>
+      <c r="B149" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_1_2017_relation</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>184</v>
-      </c>
-      <c r="B150" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_1_2018_relation</v>
+        <v>182</v>
+      </c>
+      <c r="B150" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_2_2017_relation</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>185</v>
-      </c>
-      <c r="B151" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_2_2018_relation</v>
+        <v>183</v>
+      </c>
+      <c r="B151" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_0_2018_relation</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>186</v>
-      </c>
-      <c r="B152" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_0_2019_relation</v>
+        <v>184</v>
+      </c>
+      <c r="B152" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_1_2018_relation</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>187</v>
-      </c>
-      <c r="B153" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_1_2019_relation</v>
+        <v>185</v>
+      </c>
+      <c r="B153" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_2_2018_relation</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>188</v>
-      </c>
-      <c r="B154" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_2_2019_relation</v>
+        <v>186</v>
+      </c>
+      <c r="B154" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_0_2019_relation</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>189</v>
-      </c>
-      <c r="B155" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_3_2019_relation</v>
+        <v>187</v>
+      </c>
+      <c r="B155" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_1_2019_relation</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>190</v>
-      </c>
-      <c r="B156" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_0_2020_relation</v>
+        <v>188</v>
+      </c>
+      <c r="B156" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_2_2019_relation</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>191</v>
-      </c>
-      <c r="B157" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_1_2020_relation</v>
+        <v>189</v>
+      </c>
+      <c r="B157" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_3_2019_relation</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>192</v>
-      </c>
-      <c r="B158" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_2_2020_relation</v>
+        <v>190</v>
+      </c>
+      <c r="B158" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_0_2020_relation</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>193</v>
-      </c>
-      <c r="B159" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_3_2020_relation</v>
+        <v>191</v>
+      </c>
+      <c r="B159" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_1_2020_relation</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>217</v>
-      </c>
-      <c r="B160" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>engine</v>
+        <v>192</v>
+      </c>
+      <c r="B160" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_2_2020_relation</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>218</v>
-      </c>
-      <c r="B161" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>app</v>
+        <v>193</v>
+      </c>
+      <c r="B161" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_3_2020_relation</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B162" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>client</v>
+        <v>engine</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B163" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>db</v>
+        <v>app</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B164" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>session</v>
+        <v>client</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B165" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>fiscalYears_relation</v>
+        <v>db</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B166" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>annualStatistics_relation</v>
+        <v>session</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>224</v>
-      </c>
-      <c r="B167" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendors_relation</v>
+        <v>222</v>
+      </c>
+      <c r="B167" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>fiscalYears_relation</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>225</v>
-      </c>
-      <c r="B168" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendorNotes_relation</v>
+        <v>223</v>
+      </c>
+      <c r="B168" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>annualStatistics_relation</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>226</v>
-      </c>
-      <c r="B169" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsSources_relation</v>
+        <v>224</v>
+      </c>
+      <c r="B169" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>vendors_relation</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>227</v>
-      </c>
-      <c r="B170" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsSourceNotes_relation</v>
+        <v>225</v>
+      </c>
+      <c r="B170" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>vendorNotes_relation</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>228</v>
-      </c>
-      <c r="B171" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>resourceSources_relation</v>
+        <v>226</v>
+      </c>
+      <c r="B171" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsSources_relation</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>229</v>
-      </c>
-      <c r="B172" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>resourceSourceNotes_relation</v>
+        <v>227</v>
+      </c>
+      <c r="B172" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsSourceNotes_relation</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>230</v>
-      </c>
-      <c r="B173" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsResourceSources_relation</v>
+        <v>228</v>
+      </c>
+      <c r="B173" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>resourceSources_relation</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>231</v>
-      </c>
-      <c r="B174" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>annualUsageCollectionTracking_relation</v>
+        <v>229</v>
+      </c>
+      <c r="B174" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>resourceSourceNotes_relation</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>232</v>
-      </c>
-      <c r="B175" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_0_2017_relation</v>
+        <v>230</v>
+      </c>
+      <c r="B175" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsResourceSources_relation</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>233</v>
-      </c>
-      <c r="B176" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_1_2017_relation</v>
+        <v>231</v>
+      </c>
+      <c r="B176" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>annualUsageCollectionTracking_relation</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>234</v>
-      </c>
-      <c r="B177" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_2_2017_relation</v>
+        <v>232</v>
+      </c>
+      <c r="B177" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_0_2017_relation</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>235</v>
-      </c>
-      <c r="B178" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_0_2018_relation</v>
+        <v>233</v>
+      </c>
+      <c r="B178" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_1_2017_relation</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>236</v>
-      </c>
-      <c r="B179" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_1_2018_relation</v>
+        <v>234</v>
+      </c>
+      <c r="B179" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_2_2017_relation</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>237</v>
-      </c>
-      <c r="B180" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_2_2018_relation</v>
+        <v>235</v>
+      </c>
+      <c r="B180" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_0_2018_relation</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>238</v>
-      </c>
-      <c r="B181" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_0_2019_relation</v>
+        <v>236</v>
+      </c>
+      <c r="B181" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_1_2018_relation</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>239</v>
-      </c>
-      <c r="B182" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_1_2019_relation</v>
+        <v>237</v>
+      </c>
+      <c r="B182" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_2_2018_relation</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>240</v>
-      </c>
-      <c r="B183" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_2_2019_relation</v>
+        <v>238</v>
+      </c>
+      <c r="B183" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_0_2019_relation</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>241</v>
-      </c>
-      <c r="B184" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_3_2019_relation</v>
+        <v>239</v>
+      </c>
+      <c r="B184" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_1_2019_relation</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>242</v>
-      </c>
-      <c r="B185" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_0_2020_relation</v>
+        <v>240</v>
+      </c>
+      <c r="B185" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_2_2019_relation</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>243</v>
-      </c>
-      <c r="B186" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_1_2020_relation</v>
+        <v>241</v>
+      </c>
+      <c r="B186" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_3_2019_relation</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>244</v>
-      </c>
-      <c r="B187" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_2_2020_relation</v>
+        <v>242</v>
+      </c>
+      <c r="B187" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_0_2020_relation</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>245</v>
-      </c>
-      <c r="B188" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_3_2020_relation</v>
+        <v>243</v>
+      </c>
+      <c r="B188" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_1_2020_relation</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>246</v>
-      </c>
-      <c r="B189" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbooks_and_relations</v>
+        <v>244</v>
+      </c>
+      <c r="B189" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_2_2020_relation</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>247</v>
-      </c>
-      <c r="B190" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_COUNTERData_workbook_iterdir_list</v>
+        <v>245</v>
+      </c>
+      <c r="B190" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_3_2020_relation</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B191" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>COUNTERData_relation</v>
+        <v>workbooks_and_relations</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B192" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>download_destination</v>
+        <v>create_COUNTERData_workbook_iterdir_list</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B193" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>path_to_sample_file</v>
+        <v>COUNTERData_relation</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B194" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>remove_file_from_S3</v>
+        <v>download_destination</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B195" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>non_COUNTER_AUCT_object_before_upload</v>
+        <v>path_to_sample_file</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B196" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>non_COUNTER_AUCT_object_after_upload</v>
+        <v>remove_file_from_S3</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B197" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>non_COUNTER_file_to_download_from_S3</v>
+        <v>non_COUNTER_AUCT_object_before_upload</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B198" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>header_value</v>
+        <v>non_COUNTER_AUCT_object_after_upload</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B199" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>most_recent_month_with_usage</v>
+        <v>non_COUNTER_file_to_download_from_S3</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B200" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>match_direct_SUSHI_harvest_result</v>
+        <v>header_value</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B201" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>COUNTER_reports_offered_by_statistics_source</v>
+        <v>most_recent_month_with_usage</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B202" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>prepare_HTML_page_for_comparison</v>
+        <v>match_direct_SUSHI_harvest_result</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B203" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_add_annual_statistic_value</v>
+        <v>COUNTER_reports_offered_by_statistics_source</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B204" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>AUCT_fixture_for_SUSHI</v>
+        <v>prepare_HTML_page_for_comparison</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B205" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>harvest_R5_SUSHI_result</v>
+        <v>test_add_annual_statistic_value</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B206" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_collect_annual_usage_statistics</v>
+        <v>AUCT_fixture_for_SUSHI</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B207" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_FileStorage_object</v>
+        <v>harvest_R5_SUSHI_result</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B208" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_upload_nonstandard_usage_file</v>
+        <v>test_collect_annual_usage_statistics</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B209" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_download_nonstandard_usage_file</v>
+        <v>sample_FileStorage_object</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B210" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_flask_app_creation</v>
+        <v>test_upload_nonstandard_usage_file</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B211" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_flask_client_creation</v>
+        <v>test_download_nonstandard_usage_file</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B212" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_SQLAlchemy_engine_creation</v>
+        <v>test_flask_app_creation</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B213" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_homepage</v>
+        <v>test_flask_client_creation</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B214" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_404_page</v>
+        <v>test_SQLAlchemy_engine_creation</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B215" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_load_data_into_database</v>
+        <v>test_homepage</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B216" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_query_database</v>
+        <v>test_404_page</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B217" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_loading_connected_data_into_other_relation</v>
+        <v>test_load_data_into_database</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B218" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_download_file</v>
+        <v>test_query_database</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B219" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_first_new_PK_value</v>
+        <v>test_loading_connected_data_into_other_relation</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B220" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_change_single_field_dataframe_into_series</v>
+        <v>test_download_file</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B221" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_restore_boolean_values_to_boolean_field</v>
+        <v>test_first_new_PK_value</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B222" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_upload_file_to_S3_bucket</v>
+        <v>test_change_single_field_dataframe_into_series</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B223" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_AUCT_SelectField_options</v>
+        <v>test_restore_boolean_values_to_boolean_field</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B224" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_truncate_longer_lines</v>
+        <v>test_upload_file_to_S3_bucket</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B225" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendors_relation_after_test_update_database</v>
+        <v>test_create_AUCT_SelectField_options</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B226" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_update_database</v>
+        <v>test_truncate_longer_lines</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B227" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendors_relation_after_test_update_database_with_insert_statement</v>
+        <v>vendors_relation_after_test_update_database</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B228" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_update_database_with_insert_statement</v>
+        <v>test_update_database</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B229" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_prepare_HTML_page_for_comparison</v>
+        <v>vendors_relation_after_test_update_database_with_insert_statement</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B230" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>file_name_stem_and_data</v>
+        <v>test_update_database_with_insert_statement</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B231" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_save_unconverted_data_via_upload</v>
+        <v>test_prepare_HTML_page_for_comparison</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B232" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_ISSN_regex</v>
+        <v>file_name_stem_and_data</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B233" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_ISBN_regex</v>
+        <v>test_save_unconverted_data_via_upload</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B234" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_last_day_of_month</v>
+        <v>test_ISSN_regex</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B235" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_extract_value_from_single_value_df</v>
+        <v>test_ISBN_regex</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B236" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_AWS_timestamp_format</v>
+        <v>test_last_day_of_month</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B237" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_non_COUNTER_file_name_regex</v>
+        <v>test_extract_value_from_single_value_df</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B238" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_empty_string_regex</v>
+        <v>test_AWS_timestamp_format</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B239" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_annual_stats_homepage</v>
+        <v>test_non_COUNTER_file_name_regex</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B240" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_show_fiscal_year_details</v>
+        <v>test_empty_string_regex</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B241" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_show_fiscal_year_details_submitting_RunAnnualStatsMethodsForm</v>
+        <v>test_GET_request_for_annual_stats_homepage</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B242" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_show_fiscal_year_details_submitting_EditFiscalYearForm</v>
+        <v>test_GET_request_for_show_fiscal_year_details</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B243" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_show_fiscal_year_details_submitting_EditAUCTForm</v>
+        <v>test_show_fiscal_year_details_submitting_RunAnnualStatsMethodsForm</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B244" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_ingest_usage_homepage</v>
+        <v>test_show_fiscal_year_details_submitting_EditFiscalYearForm</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B245" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_upload_COUNTER_data_via_Excel</v>
+        <v>test_show_fiscal_year_details_submitting_EditAUCTForm</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B246" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_upload_COUNTER_data_via_SQL_insert</v>
+        <v>test_ingest_usage_homepage</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B247" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_match_direct_SUSHI_harvest_result</v>
+        <v>test_upload_COUNTER_data_via_Excel</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B248" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_harvest_SUSHI_statistics</v>
+        <v>test_upload_COUNTER_data_via_SQL_insert</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B249" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_harvest_SUSHI_statistics</v>
+        <v>test_match_direct_SUSHI_harvest_result</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B250" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_upload_non_COUNTER_reports</v>
+        <v>test_GET_request_for_harvest_SUSHI_statistics</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B251" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_upload_non_COUNTER_reports</v>
+        <v>test_harvest_SUSHI_statistics</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B252" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>blank_annualUsageCollectionTracking_data_types</v>
+        <v>test_GET_request_for_upload_non_COUNTER_reports</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B253" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_fiscalYears_CSV_file</v>
+        <v>test_upload_non_COUNTER_reports</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B254" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_annualStatistics_CSV_file</v>
+        <v>blank_annualUsageCollectionTracking_data_types</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B255" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_vendors_CSV_file</v>
+        <v>create_fiscalYears_CSV_file</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B256" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_vendorNotes_CSV_file</v>
+        <v>create_annualStatistics_CSV_file</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B257" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_statisticsSources_CSV_file</v>
+        <v>create_vendors_CSV_file</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B258" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_statisticsSourceNotes_CSV_file</v>
+        <v>create_vendorNotes_CSV_file</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B259" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_resourceSources_CSV_file</v>
+        <v>create_statisticsSources_CSV_file</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B260" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_resourceSourceNotes_CSV_file</v>
+        <v>create_statisticsSourceNotes_CSV_file</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B261" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_statisticsResourceSources_CSV_file</v>
+        <v>create_resourceSources_CSV_file</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B262" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_blank_annualUsageCollectionTracking_CSV_file</v>
+        <v>create_resourceSourceNotes_CSV_file</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B263" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_annualUsageCollectionTracking_CSV_file</v>
+        <v>create_statisticsResourceSources_CSV_file</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B264" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_collect_FY_and_vendor_data</v>
+        <v>create_blank_annualUsageCollectionTracking_CSV_file</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B265" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_collect_FY_and_vendor_data</v>
+        <v>create_annualUsageCollectionTracking_CSV_file</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B266" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_collect_sources_data</v>
+        <v>test_GET_request_for_collect_FY_and_vendor_data</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B267" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_collect_AUCT_and_historical_COUNTER_data</v>
+        <v>test_collect_FY_and_vendor_data</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B268" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_collect_AUCT_and_historical_COUNTER_data</v>
+        <v>test_collect_sources_data</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B269" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_upload_historical_non_COUNTER_usage</v>
+        <v>test_GET_request_for_collect_AUCT_and_historical_COUNTER_data</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B270" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>"files_for_test_upload_historical_non_COUNTER_usage._files_for_test_upload_historical_non_COUNTER_usage"</v>
+        <v>test_collect_AUCT_and_historical_COUNTER_data</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B271" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_upload_historical_non_COUNTER_usage</v>
+        <v>test_GET_request_for_upload_historical_non_COUNTER_usage</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B272" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_login_homepage</v>
+        <v>"files_for_test_upload_historical_non_COUNTER_usage._files_for_test_upload_historical_non_COUNTER_usage"</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B273" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_logging_in</v>
+        <v>test_upload_historical_non_COUNTER_usage</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B274" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_logging_in_as_admin</v>
+        <v>test_login_homepage</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B275" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_creating_an_account</v>
+        <v>test_logging_in</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B276" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_view_lists_homepage</v>
+        <v>test_logging_in_as_admin</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B277" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_view_list_record</v>
+        <v>test_creating_an_account</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B278" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_view_list_record</v>
+        <v>test_view_lists_homepage</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B279" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_edit_list_record_for_existing_record</v>
+        <v>test_GET_request_for_view_list_record</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B280" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_edit_list_record_for_new_record</v>
+        <v>test_view_list_record</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B281" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_edit_list_record</v>
+        <v>test_GET_request_for_edit_list_record_for_existing_record</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B282" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>COUNTER_download_CSV</v>
+        <v>test_GET_request_for_edit_list_record_for_new_record</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B283" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_COUNTER_fixed_vocab_list</v>
+        <v>test_edit_list_record</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B284" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_set_encoding</v>
+        <v>COUNTER_download_CSV</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B285" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_view_usage_homepage</v>
+        <v>test_create_COUNTER_fixed_vocab_list</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B286" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_run_custom_SQL_query</v>
+        <v>test_set_encoding</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B287" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_use_predefined_SQL_query</v>
+        <v>test_view_usage_homepage</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B288" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>start_query_wizard_form_data</v>
+        <v>test_run_custom_SQL_query</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B289" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_start_query_wizard</v>
+        <v>test_use_predefined_SQL_query</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B290" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_query_wizard_sort_redirect</v>
+        <v>start_query_wizard_form_data</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B291" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>PR_parameters</v>
+        <v>test_start_query_wizard</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B292" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_construct_PR_query_with_wizard</v>
+        <v>test_GET_query_wizard_sort_redirect</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B293" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>DR_parameters</v>
+        <v>PR_parameters</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B294" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_construct_DR_query_with_wizard</v>
+        <v>test_construct_PR_query_with_wizard</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B295" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>TR_parameters</v>
+        <v>DR_parameters</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B296" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_construct_TR_query_with_wizard</v>
+        <v>test_construct_DR_query_with_wizard</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B297" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>IR_parameters</v>
+        <v>TR_parameters</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B298" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_construct_IR_query_with_wizard</v>
+        <v>test_construct_TR_query_with_wizard</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B299" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>construct_PR_query_with_wizard_without_string_match</v>
+        <v>IR_parameters</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B300" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_download_non_COUNTER_usage</v>
+        <v>test_construct_IR_query_with_wizard</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B301" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_download_non_COUNTER_usage</v>
+        <v>construct_PR_query_with_wizard_without_string_match</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B302" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_PR_response_R5_JSON_dict</v>
+        <v>test_GET_request_for_download_non_COUNTER_usage</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B303" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_PR_response_R5_dataframe</v>
+        <v>test_download_non_COUNTER_usage</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B304" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_DR_response_R5_JSON_dict</v>
+        <v>sample_SUSHI_PR_response_R5_JSON_dict</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B305" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_DR_response_R5_dataframe</v>
+        <v>sample_SUSHI_PR_response_R5_dataframe</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B306" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_TR_response_R5_JSON_dict</v>
+        <v>sample_SUSHI_DR_response_R5_JSON_dict</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B307" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_TR_response_R5_dataframe</v>
+        <v>sample_SUSHI_DR_response_R5_dataframe</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B308" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_IR_response_R5_JSON_dict</v>
+        <v>sample_SUSHI_TR_response_R5_JSON_dict</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B309" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_IR_response_R5_dataframe</v>
+        <v>sample_SUSHI_TR_response_R5_dataframe</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B310" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_PR_response_R5b1_JSON_dict</v>
+        <v>sample_SUSHI_IR_response_R5_JSON_dict</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B311" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_PR_response_R5b1_dataframe</v>
+        <v>sample_SUSHI_IR_response_R5_dataframe</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B312" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_DR_response_R5b1_JSON_dict</v>
+        <v>sample_SUSHI_PR_response_R5b1_JSON_dict</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B313" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_DR_response_R5b1_dataframe</v>
+        <v>sample_SUSHI_PR_response_R5b1_dataframe</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B314" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_TR_response_R5b1_JSON_dict</v>
+        <v>sample_SUSHI_DR_response_R5b1_JSON_dict</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B315" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_TR_response_R5b1_dataframe</v>
+        <v>sample_SUSHI_DR_response_R5b1_dataframe</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B316" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_IR_response_R5b1_JSON_dict</v>
+        <v>sample_SUSHI_TR_response_R5b1_JSON_dict</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B317" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_IR_response_R5b1_dataframe</v>
+        <v>sample_SUSHI_TR_response_R5b1_dataframe</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B318" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5_PR</v>
+        <v>sample_SUSHI_IR_response_R5b1_JSON_dict</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B319" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5_DR</v>
+        <v>sample_SUSHI_IR_response_R5b1_dataframe</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B320" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5_TR</v>
+        <v>test_create_dataframe_from_R5_PR</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B321" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5_IR</v>
+        <v>test_create_dataframe_from_R5_DR</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B322" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5b1_PR</v>
+        <v>test_create_dataframe_from_R5_TR</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B323" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5b1_DR</v>
+        <v>test_create_dataframe_from_R5_IR</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B324" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5b1_TR</v>
+        <v>test_create_dataframe_from_R5b1_PR</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B325" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5b1_IR</v>
+        <v>test_create_dataframe_from_R5b1_DR</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B326" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>FY2020_FiscalYears_object</v>
+        <v>test_create_dataframe_from_R5b1_TR</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B327" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_depreciated_ACRL_60b</v>
+        <v>test_create_dataframe_from_R5b1_IR</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B328" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_depreciated_ACRL_63</v>
+        <v>FY2020_FiscalYears_object</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B329" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_ACRL_61a</v>
+        <v>test_calculate_depreciated_ACRL_60b</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B330" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_ACRL_61b</v>
+        <v>test_calculate_depreciated_ACRL_63</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B331" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_ARL_18</v>
+        <v>test_calculate_ACRL_61a</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B332" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_ARL_19</v>
+        <v>test_calculate_ACRL_61b</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B333" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_ARL_20</v>
+        <v>test_calculate_ARL_18</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B334" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>FY2023_FiscalYears_object_and_record</v>
+        <v>test_calculate_ARL_19</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B335" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>load_new_record_into_fiscalYears</v>
+        <v>test_calculate_ARL_20</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B336" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_usage_tracking_records_for_fiscal_year</v>
+        <v>FY2023_FiscalYears_object_and_record</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B337" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>FY2022_FiscalYears_object</v>
+        <v>load_new_record_into_fiscalYears</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>4</v>
+        <v>406</v>
       </c>
       <c r="B338" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_collect_fiscal_year_usage_statistics</v>
+        <v>test_create_usage_tracking_records_for_fiscal_year</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B339" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_add_access_stop_date</v>
+        <v>FY2022_FiscalYears_object</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>410</v>
+        <v>4</v>
       </c>
       <c r="B340" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_remove_access_stop_date</v>
+        <v>test_collect_fiscal_year_usage_statistics</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B341" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_change_StatisticsSource</v>
+        <v>test_add_access_stop_date</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B342" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_add_note</v>
+        <v>test_remove_access_stop_date</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B343" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_format_list_for_stdout_with_list</v>
+        <v>test_change_StatisticsSource</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>415</v>
-      </c>
-      <c r="B344" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_format_list_for_stdout_with_generator</v>
+        <v>412</v>
+      </c>
+      <c r="B344" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_add_note</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B345" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_remove_IDE_spacing_from_statement</v>
+        <v>test_format_list_for_stdout_with_list</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B346" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>current_month_like_most_recent_month_with_usage</v>
+        <v>test_format_list_for_stdout_with_generator</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>5</v>
+        <v>416</v>
       </c>
       <c r="B347" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>StatisticsSources_fixture</v>
+        <v>test_remove_IDE_spacing_from_statement</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B348" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_fetch_SUSHI_information_for_API</v>
+        <v>current_month_like_most_recent_month_with_usage</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>420</v>
+        <v>5</v>
       </c>
       <c r="B349" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_fetch_SUSHI_information_for_display</v>
+        <v>StatisticsSources_fixture</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B350" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>SUSHI_credentials_fixture</v>
+        <v>test_fetch_SUSHI_information_for_API</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B351" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>reports_offered_by_StatisticsSource_fixture</v>
+        <v>test_fetch_SUSHI_information_for_display</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>423</v>
-      </c>
-      <c r="B352" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_COUNTER_reports_offered_by_statistics_source</v>
+        <v>421</v>
+      </c>
+      <c r="B352" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>SUSHI_credentials_fixture</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B353" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_check_if_data_in_database_no</v>
+        <v>reports_offered_by_StatisticsSource_fixture</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B354" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_check_if_data_in_database_yes</v>
+        <v>test_COUNTER_reports_offered_by_statistics_source</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B355" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_harvest_single_report</v>
+        <v>test_check_if_data_in_database_no</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B356" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_harvest_single_report_with_partial_date_range</v>
+        <v>test_check_if_data_in_database_yes</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B357" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_harvest_R5_SUSHI</v>
+        <v>test_harvest_single_report</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B358" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_harvest_R5_SUSHI_with_report_to_harvest</v>
+        <v>test_harvest_single_report_with_partial_date_range</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B359" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_harvest_R5_SUSHI_with_invalid_dates</v>
+        <v>test_harvest_R5_SUSHI</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B360" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>month_before_month_like_most_recent_month_with_usage</v>
+        <v>test_harvest_R5_SUSHI_with_report_to_harvest</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B361" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>harvest_R5_SUSHI_result_in_test_StatisticsSources</v>
+        <v>test_harvest_R5_SUSHI_with_invalid_dates</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B362" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_collect_usage_statistics</v>
+        <v>month_before_month_like_most_recent_month_with_usage</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B363" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_add_note</v>
+        <v>harvest_R5_SUSHI_result_in_test_StatisticsSources</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B364" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>partially_duplicate_COUNTER_data</v>
+        <v>test_collect_usage_statistics</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>436</v>
-      </c>
-      <c r="B365" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>non_duplicate_COUNTER_data</v>
+        <v>434</v>
+      </c>
+      <c r="B365" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_add_note</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B366" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_check_if_data_already_in_COUNTERData</v>
+        <v>partially_duplicate_COUNTER_data</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B367" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>SUSHI_credentials_fixture</v>
+        <v>non_duplicate_COUNTER_data</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B368" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>StatisticsSource_instance_name</v>
+        <v>test_check_if_data_already_in_COUNTERData</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>442</v>
-      </c>
-      <c r="B369" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_status_call</v>
+        <v>439</v>
+      </c>
+      <c r="B369" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>SUSHI_credentials_fixture</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B370" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_status_call_validity</v>
+        <v>StatisticsSource_instance_name</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B371" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_reports_call</v>
+        <v>test_status_call</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B372" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_reports_call_validity</v>
+        <v>test_status_call_validity</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B373" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>list_of_reports</v>
+        <v>test_reports_call</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B374" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_PR_call_validity</v>
+        <v>test_reports_call_validity</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B375" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_DR_call_validity</v>
+        <v>list_of_reports</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B376" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_TR_call_validity</v>
+        <v>test_PR_call_validity</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B377" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_IR_call_validity</v>
+        <v>test_DR_call_validity</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B378" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_call_with_invalid_credentials</v>
+        <v>test_TR_call_validity</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B379" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_COUNTER_report_workbook</v>
+        <v>test_IR_call_validity</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B380" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_single_workbook</v>
+        <v>test_call_with_invalid_credentials</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B381" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_COUNTER_report_workbooks</v>
+        <v>sample_COUNTER_report_workbook</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B382" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe</v>
+        <v>test_create_dataframe_from_single_workbook</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B383" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_get_statisticsSources_records</v>
+        <v>sample_COUNTER_report_workbooks</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B384" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_get_resourceSources_records</v>
+        <v>test_create_dataframe</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
+        <v>458</v>
+      </c>
+      <c r="B385" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_get_statisticsSources_records</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A386" t="s">
+        <v>459</v>
+      </c>
+      <c r="B386" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_get_resourceSources_records</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A387" t="s">
         <v>460</v>
       </c>
-      <c r="B385" t="str">
+      <c r="B387" s="2" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
         <v>test_add_note</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B385">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Update call chain workbook again
</commit_message>
<xml_diff>
--- a/docs/source/function_call_chain_connections.xlsx
+++ b/docs/source/function_call_chain_connections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereiskind\nolcat\docs\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CB3833-B5D9-4B1D-BF3D-04AE9EE3FEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8D3636-F9A4-4CCB-B6BC-F7C16F9C0F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{44512B9D-2A90-4646-8933-428A99F14C9B}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2933" uniqueCount="466">
   <si>
     <t>Called Function</t>
   </si>
@@ -1523,9 +1523,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1542,6 +1539,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1565,14 +1565,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A35B55CA-3D7A-4630-80A4-302CC6486C4B}" name="Table3" displayName="Table3" ref="A1:D946" totalsRowShown="0">
-  <autoFilter ref="A1:D946" xr:uid="{A35B55CA-3D7A-4630-80A4-302CC6486C4B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A35B55CA-3D7A-4630-80A4-302CC6486C4B}" name="Table3" displayName="Table3" ref="A1:D997" totalsRowShown="0">
+  <autoFilter ref="A1:D997" xr:uid="{A35B55CA-3D7A-4630-80A4-302CC6486C4B}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7FD1105F-C7A5-4E16-926A-A61CDD080060}" name="Called Node Name"/>
     <tableColumn id="2" xr3:uid="{CE4DE19D-EA52-4CF0-9B0C-C1DFDE7DD080}" name="Called Function" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E906BA6C-7812-4693-8C6F-E4D00CFF9BC1}" name="Check" dataDxfId="1" dataCellStyle="Normal">
+    <tableColumn id="4" xr3:uid="{E906BA6C-7812-4693-8C6F-E4D00CFF9BC1}" name="Check" dataDxfId="3" dataCellStyle="Normal">
       <calculatedColumnFormula>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{C2024EA6-7D5C-4C8B-9CCD-AF563856B1E1}" name="Calling Node"/>
@@ -1582,13 +1582,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{71A6869D-4B7A-4FAA-A02E-10A2F1466D47}" name="Table2" displayName="Table2" ref="A1:D385" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{71A6869D-4B7A-4FAA-A02E-10A2F1466D47}" name="Table2" displayName="Table2" ref="A1:D385" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:D385" xr:uid="{A6211418-BCE9-480F-9AC5-9CD507C26481}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{69CD15C3-5B02-4859-BD05-680C3DBFC908}" name="Node Name"/>
     <tableColumn id="2" xr3:uid="{3B8ECDB6-A578-4E02-AC3C-7452D338C2BE}" name="Function Name"/>
     <tableColumn id="3" xr3:uid="{D3E5C4D2-15D2-41F6-B02F-14A3A95B3654}" name="Cluster"/>
-    <tableColumn id="4" xr3:uid="{C97D9CDF-DBD9-426B-97D0-179A8305BFF1}" name="Order Within Cluster" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{C97D9CDF-DBD9-426B-97D0-179A8305BFF1}" name="Order Within Cluster" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1911,10 +1911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202E7D9A-A4E5-4FC3-B37C-A36A5067E5D4}">
-  <dimension ref="A1:D946"/>
+  <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A680" workbookViewId="0">
-      <selection activeCell="E686" sqref="E686"/>
+    <sheetView tabSelected="1" topLeftCell="A748" workbookViewId="0">
+      <selection activeCell="D756" sqref="D756"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13073,85 +13073,136 @@
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
+      <c r="D699" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="700" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B700" t="e">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>#N/A</v>
+      <c r="A700" t="s">
+        <v>217</v>
+      </c>
+      <c r="B700" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>app</v>
       </c>
       <c r="C700" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
+      <c r="D700" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="701" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B701" t="e">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>#N/A</v>
+      <c r="A701" t="s">
+        <v>218</v>
+      </c>
+      <c r="B701" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C701" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
+      <c r="D701" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="702" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B702" t="e">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>#N/A</v>
+      <c r="A702" t="s">
+        <v>218</v>
+      </c>
+      <c r="B702" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C702" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
+      <c r="D702" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="703" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B703" t="e">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>#N/A</v>
+      <c r="A703" t="s">
+        <v>218</v>
+      </c>
+      <c r="B703" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C703" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
+      <c r="D703" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="704" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B704" t="e">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>#N/A</v>
+      <c r="A704" t="s">
+        <v>218</v>
+      </c>
+      <c r="B704" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C704" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
+      <c r="D704" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="705" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B705" t="e">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>#N/A</v>
+      <c r="A705" t="s">
+        <v>218</v>
+      </c>
+      <c r="B705" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C705" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
+      <c r="D705" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="706" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B706" t="e">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>#N/A</v>
+      <c r="A706" t="s">
+        <v>218</v>
+      </c>
+      <c r="B706" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C706" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
+      <c r="D706" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="707" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B707" t="e">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>#N/A</v>
+      <c r="A707" t="s">
+        <v>218</v>
+      </c>
+      <c r="B707" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C707" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
+      </c>
+      <c r="D707" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="708" spans="1:4" x14ac:dyDescent="0.3">
@@ -13166,1302 +13217,1443 @@
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
+      <c r="D708" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="709" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A709" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B709" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>db</v>
+        <v>client</v>
       </c>
       <c r="C709" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
+      </c>
+      <c r="D709" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="710" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A710" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B710" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>session</v>
+        <v>client</v>
       </c>
       <c r="C710" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
+      </c>
+      <c r="D710" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="711" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A711" t="s">
-        <v>221</v>
-      </c>
-      <c r="B711" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>fiscalYears_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B711" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C711" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D711" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="712" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A712" t="s">
-        <v>221</v>
-      </c>
-      <c r="B712" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>fiscalYears_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B712" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C712" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D712" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
     </row>
     <row r="713" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A713" t="s">
-        <v>222</v>
-      </c>
-      <c r="B713" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>annualStatistics_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B713" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C713" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D713" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="714" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A714" t="s">
-        <v>222</v>
-      </c>
-      <c r="B714" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>annualStatistics_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B714" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C714" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D714" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
     </row>
     <row r="715" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A715" t="s">
-        <v>223</v>
-      </c>
-      <c r="B715" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendors_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B715" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C715" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D715" t="s">
-        <v>275</v>
+        <v>327</v>
       </c>
     </row>
     <row r="716" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A716" t="s">
-        <v>223</v>
-      </c>
-      <c r="B716" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendors_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B716" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C716" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D716" t="s">
-        <v>276</v>
+        <v>328</v>
       </c>
     </row>
     <row r="717" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A717" t="s">
-        <v>223</v>
-      </c>
-      <c r="B717" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendors_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B717" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C717" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D717" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
     </row>
     <row r="718" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A718" t="s">
-        <v>223</v>
-      </c>
-      <c r="B718" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendors_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B718" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C718" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D718" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="719" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A719" t="s">
-        <v>224</v>
-      </c>
-      <c r="B719" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendorNotes_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B719" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C719" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D719" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
     </row>
     <row r="720" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A720" t="s">
-        <v>224</v>
-      </c>
-      <c r="B720" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendorNotes_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B720" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C720" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D720" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="721" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A721" t="s">
-        <v>225</v>
-      </c>
-      <c r="B721" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsSources_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B721" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C721" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D721" t="s">
-        <v>277</v>
+        <v>335</v>
       </c>
     </row>
     <row r="722" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A722" t="s">
-        <v>225</v>
-      </c>
-      <c r="B722" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsSources_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B722" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C722" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D722" t="s">
-        <v>320</v>
+        <v>337</v>
       </c>
     </row>
     <row r="723" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A723" t="s">
-        <v>225</v>
-      </c>
-      <c r="B723" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsSources_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B723" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C723" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D723" t="s">
-        <v>329</v>
+        <v>352</v>
       </c>
     </row>
     <row r="724" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A724" t="s">
-        <v>226</v>
-      </c>
-      <c r="B724" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsSourceNotes_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B724" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C724" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D724" t="s">
-        <v>321</v>
+        <v>353</v>
       </c>
     </row>
     <row r="725" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A725" t="s">
-        <v>226</v>
-      </c>
-      <c r="B725" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsSourceNotes_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B725" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C725" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D725" t="s">
-        <v>329</v>
+        <v>354</v>
       </c>
     </row>
     <row r="726" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A726" t="s">
-        <v>227</v>
-      </c>
-      <c r="B726" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>resourceSources_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B726" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C726" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D726" t="s">
-        <v>322</v>
+        <v>356</v>
       </c>
     </row>
     <row r="727" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A727" t="s">
-        <v>227</v>
-      </c>
-      <c r="B727" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>resourceSources_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B727" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C727" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D727" t="s">
-        <v>329</v>
+        <v>357</v>
       </c>
     </row>
     <row r="728" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A728" t="s">
-        <v>228</v>
-      </c>
-      <c r="B728" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>resourceSourceNotes_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B728" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C728" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D728" t="s">
-        <v>323</v>
+        <v>359</v>
       </c>
     </row>
     <row r="729" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A729" t="s">
-        <v>228</v>
-      </c>
-      <c r="B729" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>resourceSourceNotes_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B729" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C729" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D729" t="s">
-        <v>329</v>
+        <v>361</v>
       </c>
     </row>
     <row r="730" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A730" t="s">
-        <v>229</v>
-      </c>
-      <c r="B730" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsResourceSources_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B730" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C730" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D730" t="s">
-        <v>324</v>
+        <v>363</v>
       </c>
     </row>
     <row r="731" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A731" t="s">
-        <v>229</v>
-      </c>
-      <c r="B731" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>statisticsResourceSources_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B731" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C731" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D731" t="s">
-        <v>329</v>
+        <v>365</v>
       </c>
     </row>
     <row r="732" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A732" t="s">
-        <v>230</v>
-      </c>
-      <c r="B732" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>annualUsageCollectionTracking_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B732" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C732" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D732" t="s">
-        <v>326</v>
+        <v>367</v>
       </c>
     </row>
     <row r="733" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A733" t="s">
-        <v>230</v>
-      </c>
-      <c r="B733" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>annualUsageCollectionTracking_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B733" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C733" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D733" t="s">
-        <v>331</v>
+        <v>368</v>
       </c>
     </row>
     <row r="734" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A734" t="s">
-        <v>231</v>
-      </c>
-      <c r="B734" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_0_2017_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B734" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C734" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D734" t="s">
-        <v>245</v>
+        <v>396</v>
       </c>
     </row>
     <row r="735" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A735" t="s">
-        <v>232</v>
-      </c>
-      <c r="B735" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_1_2017_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B735" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C735" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D735" t="s">
-        <v>245</v>
+        <v>397</v>
       </c>
     </row>
     <row r="736" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A736" t="s">
-        <v>233</v>
-      </c>
-      <c r="B736" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_2_2017_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B736" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C736" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D736" t="s">
-        <v>245</v>
+        <v>398</v>
       </c>
     </row>
     <row r="737" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A737" t="s">
-        <v>234</v>
-      </c>
-      <c r="B737" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_0_2018_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B737" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C737" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D737" t="s">
-        <v>245</v>
+        <v>399</v>
       </c>
     </row>
     <row r="738" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A738" t="s">
-        <v>235</v>
-      </c>
-      <c r="B738" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_1_2018_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B738" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C738" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D738" t="s">
-        <v>245</v>
+        <v>400</v>
       </c>
     </row>
     <row r="739" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A739" t="s">
-        <v>236</v>
-      </c>
-      <c r="B739" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_2_2018_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B739" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C739" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D739" t="s">
-        <v>245</v>
+        <v>401</v>
       </c>
     </row>
     <row r="740" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A740" t="s">
-        <v>237</v>
-      </c>
-      <c r="B740" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_0_2019_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B740" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C740" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D740" t="s">
-        <v>245</v>
+        <v>402</v>
       </c>
     </row>
     <row r="741" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A741" t="s">
-        <v>238</v>
-      </c>
-      <c r="B741" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_1_2019_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B741" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C741" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D741" t="s">
-        <v>245</v>
+        <v>405</v>
       </c>
     </row>
     <row r="742" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A742" t="s">
-        <v>239</v>
-      </c>
-      <c r="B742" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_2_2019_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B742" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C742" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D742" t="s">
-        <v>245</v>
+        <v>423</v>
       </c>
     </row>
     <row r="743" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A743" t="s">
-        <v>240</v>
-      </c>
-      <c r="B743" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_3_2019_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B743" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C743" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D743" t="s">
-        <v>245</v>
+        <v>424</v>
       </c>
     </row>
     <row r="744" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A744" t="s">
-        <v>241</v>
-      </c>
-      <c r="B744" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_0_2020_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B744" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C744" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D744" t="s">
-        <v>245</v>
+        <v>425</v>
       </c>
     </row>
     <row r="745" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A745" t="s">
-        <v>242</v>
-      </c>
-      <c r="B745" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_1_2020_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B745" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C745" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D745" t="s">
-        <v>245</v>
+        <v>426</v>
       </c>
     </row>
     <row r="746" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A746" t="s">
-        <v>243</v>
-      </c>
-      <c r="B746" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_2_2020_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B746" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C746" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D746" t="s">
-        <v>245</v>
+        <v>427</v>
       </c>
     </row>
     <row r="747" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A747" t="s">
-        <v>244</v>
-      </c>
-      <c r="B747" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbook_3_2020_relation</v>
+        <v>218</v>
+      </c>
+      <c r="B747" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C747" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
       <c r="D747" t="s">
-        <v>245</v>
+        <v>441</v>
       </c>
     </row>
     <row r="748" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A748" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="B748" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>workbooks_and_relations</v>
+        <v>client</v>
       </c>
       <c r="C748" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
+      <c r="D748" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="749" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B749" t="e">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>#N/A</v>
+      <c r="A749" t="s">
+        <v>218</v>
+      </c>
+      <c r="B749" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C749" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
+      <c r="D749" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="750" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B750" t="e">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>#N/A</v>
+      <c r="A750" t="s">
+        <v>218</v>
+      </c>
+      <c r="B750" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>client</v>
       </c>
       <c r="C750" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
+      </c>
+      <c r="D750" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="751" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A751" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="B751" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_COUNTERData_workbook_iterdir_list</v>
+        <v>client</v>
       </c>
       <c r="C751" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
+      </c>
+      <c r="D751" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="752" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A752" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="B752" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>COUNTERData_relation</v>
+        <v>client</v>
       </c>
       <c r="C752" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="753" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D752" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="753" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A753" t="s">
-        <v>248</v>
+        <v>218</v>
       </c>
       <c r="B753" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>download_destination</v>
+        <v>client</v>
       </c>
       <c r="C753" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="754" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D753" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="754" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A754" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
       <c r="B754" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>path_to_sample_file</v>
+        <v>client</v>
       </c>
       <c r="C754" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="755" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D754" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="755" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A755" t="s">
-        <v>250</v>
+        <v>218</v>
       </c>
       <c r="B755" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>remove_file_from_S3</v>
+        <v>client</v>
       </c>
       <c r="C755" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="756" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D755" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="756" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A756" t="s">
-        <v>251</v>
+        <v>219</v>
       </c>
       <c r="B756" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>non_COUNTER_AUCT_object_before_upload</v>
+        <v>db</v>
       </c>
       <c r="C756" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="757" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D756" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="757" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A757" t="s">
-        <v>252</v>
+        <v>220</v>
       </c>
       <c r="B757" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>non_COUNTER_AUCT_object_after_upload</v>
+        <v>session</v>
       </c>
       <c r="C757" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="758" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D757" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="758" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A758" t="s">
-        <v>253</v>
-      </c>
-      <c r="B758" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>non_COUNTER_file_to_download_from_S3</v>
+        <v>221</v>
+      </c>
+      <c r="B758" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>fiscalYears_relation</v>
       </c>
       <c r="C758" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="759" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D758" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="759" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A759" t="s">
-        <v>254</v>
-      </c>
-      <c r="B759" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>header_value</v>
+        <v>221</v>
+      </c>
+      <c r="B759" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>fiscalYears_relation</v>
       </c>
       <c r="C759" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="760" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D759" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="760" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A760" t="s">
-        <v>255</v>
-      </c>
-      <c r="B760" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>most_recent_month_with_usage</v>
+        <v>222</v>
+      </c>
+      <c r="B760" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>annualStatistics_relation</v>
       </c>
       <c r="C760" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="761" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D760" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="761" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A761" t="s">
-        <v>256</v>
-      </c>
-      <c r="B761" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>match_direct_SUSHI_harvest_result</v>
+        <v>222</v>
+      </c>
+      <c r="B761" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>annualStatistics_relation</v>
       </c>
       <c r="C761" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="762" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D761" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="762" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A762" t="s">
-        <v>257</v>
-      </c>
-      <c r="B762" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>COUNTER_reports_offered_by_statistics_source</v>
+        <v>223</v>
+      </c>
+      <c r="B762" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>vendors_relation</v>
       </c>
       <c r="C762" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="763" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D762" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="763" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A763" t="s">
-        <v>258</v>
-      </c>
-      <c r="B763" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>prepare_HTML_page_for_comparison</v>
+        <v>223</v>
+      </c>
+      <c r="B763" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>vendors_relation</v>
       </c>
       <c r="C763" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="764" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D763" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="764" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A764" t="s">
-        <v>260</v>
-      </c>
-      <c r="B764" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_add_annual_statistic_value</v>
+        <v>223</v>
+      </c>
+      <c r="B764" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>vendors_relation</v>
       </c>
       <c r="C764" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="765" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D764" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="765" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A765" t="s">
-        <v>262</v>
-      </c>
-      <c r="B765" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>AUCT_fixture_for_SUSHI</v>
+        <v>223</v>
+      </c>
+      <c r="B765" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>vendors_relation</v>
       </c>
       <c r="C765" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="766" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D765" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="766" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A766" t="s">
-        <v>263</v>
+        <v>224</v>
       </c>
       <c r="B766" s="2" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>harvest_R5_SUSHI_result</v>
+        <v>vendorNotes_relation</v>
       </c>
       <c r="C766" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="767" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D766" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="767" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A767" t="s">
-        <v>265</v>
-      </c>
-      <c r="B767" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_collect_annual_usage_statistics</v>
+        <v>224</v>
+      </c>
+      <c r="B767" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>vendorNotes_relation</v>
       </c>
       <c r="C767" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="768" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D767" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="768" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A768" t="s">
-        <v>266</v>
-      </c>
-      <c r="B768" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_FileStorage_object</v>
+        <v>225</v>
+      </c>
+      <c r="B768" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsSources_relation</v>
       </c>
       <c r="C768" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="769" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D768" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="769" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A769" t="s">
-        <v>267</v>
-      </c>
-      <c r="B769" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_upload_nonstandard_usage_file</v>
+        <v>225</v>
+      </c>
+      <c r="B769" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsSources_relation</v>
       </c>
       <c r="C769" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="770" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D769" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="770" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A770" t="s">
-        <v>268</v>
-      </c>
-      <c r="B770" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_download_nonstandard_usage_file</v>
+        <v>225</v>
+      </c>
+      <c r="B770" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsSources_relation</v>
       </c>
       <c r="C770" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="771" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D770" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="771" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A771" t="s">
-        <v>270</v>
-      </c>
-      <c r="B771" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_flask_app_creation</v>
+        <v>226</v>
+      </c>
+      <c r="B771" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsSourceNotes_relation</v>
       </c>
       <c r="C771" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="772" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D771" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="772" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A772" t="s">
-        <v>271</v>
-      </c>
-      <c r="B772" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_flask_client_creation</v>
+        <v>226</v>
+      </c>
+      <c r="B772" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsSourceNotes_relation</v>
       </c>
       <c r="C772" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="773" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D772" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="773" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A773" t="s">
-        <v>272</v>
-      </c>
-      <c r="B773" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_SQLAlchemy_engine_creation</v>
+        <v>227</v>
+      </c>
+      <c r="B773" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>resourceSources_relation</v>
       </c>
       <c r="C773" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="774" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D773" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="774" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A774" t="s">
-        <v>273</v>
-      </c>
-      <c r="B774" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_homepage</v>
+        <v>227</v>
+      </c>
+      <c r="B774" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>resourceSources_relation</v>
       </c>
       <c r="C774" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="775" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D774" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="775" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A775" t="s">
-        <v>274</v>
-      </c>
-      <c r="B775" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_404_page</v>
+        <v>228</v>
+      </c>
+      <c r="B775" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>resourceSourceNotes_relation</v>
       </c>
       <c r="C775" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="776" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D775" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="776" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A776" t="s">
-        <v>275</v>
-      </c>
-      <c r="B776" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_load_data_into_database</v>
+        <v>228</v>
+      </c>
+      <c r="B776" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>resourceSourceNotes_relation</v>
       </c>
       <c r="C776" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="777" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D776" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="777" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A777" t="s">
-        <v>276</v>
-      </c>
-      <c r="B777" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_query_database</v>
+        <v>229</v>
+      </c>
+      <c r="B777" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsResourceSources_relation</v>
       </c>
       <c r="C777" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="778" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D777" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="778" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A778" t="s">
-        <v>277</v>
-      </c>
-      <c r="B778" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_loading_connected_data_into_other_relation</v>
+        <v>229</v>
+      </c>
+      <c r="B778" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>statisticsResourceSources_relation</v>
       </c>
       <c r="C778" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="779" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D778" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="779" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A779" t="s">
-        <v>278</v>
-      </c>
-      <c r="B779" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_download_file</v>
+        <v>230</v>
+      </c>
+      <c r="B779" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>annualUsageCollectionTracking_relation</v>
       </c>
       <c r="C779" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="780" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D779" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="780" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A780" t="s">
-        <v>279</v>
-      </c>
-      <c r="B780" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_first_new_PK_value</v>
+        <v>230</v>
+      </c>
+      <c r="B780" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>annualUsageCollectionTracking_relation</v>
       </c>
       <c r="C780" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="781" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D780" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="781" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A781" t="s">
-        <v>280</v>
-      </c>
-      <c r="B781" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_change_single_field_dataframe_into_series</v>
+        <v>231</v>
+      </c>
+      <c r="B781" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_0_2017_relation</v>
       </c>
       <c r="C781" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="782" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D781" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="782" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A782" t="s">
-        <v>281</v>
-      </c>
-      <c r="B782" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_restore_boolean_values_to_boolean_field</v>
+        <v>232</v>
+      </c>
+      <c r="B782" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_1_2017_relation</v>
       </c>
       <c r="C782" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="783" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D782" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="783" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A783" t="s">
-        <v>282</v>
-      </c>
-      <c r="B783" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_upload_file_to_S3_bucket</v>
+        <v>233</v>
+      </c>
+      <c r="B783" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_2_2017_relation</v>
       </c>
       <c r="C783" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="784" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D783" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="784" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A784" t="s">
-        <v>283</v>
-      </c>
-      <c r="B784" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_AUCT_SelectField_options</v>
+        <v>234</v>
+      </c>
+      <c r="B784" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_0_2018_relation</v>
       </c>
       <c r="C784" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="785" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D784" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="785" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A785" t="s">
-        <v>284</v>
-      </c>
-      <c r="B785" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_truncate_longer_lines</v>
+        <v>235</v>
+      </c>
+      <c r="B785" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_1_2018_relation</v>
       </c>
       <c r="C785" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="786" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D785" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="786" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A786" t="s">
-        <v>285</v>
-      </c>
-      <c r="B786" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendors_relation_after_test_update_database</v>
+        <v>236</v>
+      </c>
+      <c r="B786" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_2_2018_relation</v>
       </c>
       <c r="C786" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="787" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D786" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="787" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A787" t="s">
-        <v>286</v>
-      </c>
-      <c r="B787" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_update_database</v>
+        <v>237</v>
+      </c>
+      <c r="B787" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_0_2019_relation</v>
       </c>
       <c r="C787" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="788" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D787" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="788" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A788" t="s">
-        <v>287</v>
-      </c>
-      <c r="B788" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>vendors_relation_after_test_update_database_with_insert_statement</v>
+        <v>238</v>
+      </c>
+      <c r="B788" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_1_2019_relation</v>
       </c>
       <c r="C788" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="789" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D788" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="789" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A789" t="s">
-        <v>288</v>
-      </c>
-      <c r="B789" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_update_database_with_insert_statement</v>
+        <v>239</v>
+      </c>
+      <c r="B789" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_2_2019_relation</v>
       </c>
       <c r="C789" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="790" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D789" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="790" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A790" t="s">
-        <v>289</v>
-      </c>
-      <c r="B790" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_prepare_HTML_page_for_comparison</v>
+        <v>240</v>
+      </c>
+      <c r="B790" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_3_2019_relation</v>
       </c>
       <c r="C790" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="791" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D790" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="791" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A791" t="s">
-        <v>290</v>
-      </c>
-      <c r="B791" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>file_name_stem_and_data</v>
+        <v>241</v>
+      </c>
+      <c r="B791" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_0_2020_relation</v>
       </c>
       <c r="C791" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="792" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D791" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="792" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A792" t="s">
-        <v>291</v>
-      </c>
-      <c r="B792" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_save_unconverted_data_via_upload</v>
+        <v>242</v>
+      </c>
+      <c r="B792" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_1_2020_relation</v>
       </c>
       <c r="C792" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="793" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D792" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="793" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A793" t="s">
-        <v>292</v>
-      </c>
-      <c r="B793" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_ISSN_regex</v>
+        <v>243</v>
+      </c>
+      <c r="B793" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_2_2020_relation</v>
       </c>
       <c r="C793" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="794" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D793" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="794" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A794" t="s">
-        <v>293</v>
-      </c>
-      <c r="B794" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_ISBN_regex</v>
+        <v>244</v>
+      </c>
+      <c r="B794" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>workbook_3_2020_relation</v>
       </c>
       <c r="C794" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="795" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D794" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="795" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A795" t="s">
-        <v>294</v>
+        <v>245</v>
       </c>
       <c r="B795" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_last_day_of_month</v>
+        <v>workbooks_and_relations</v>
       </c>
       <c r="C795" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="796" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A796" t="s">
-        <v>295</v>
-      </c>
-      <c r="B796" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_extract_value_from_single_value_df</v>
+    <row r="796" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B796" t="e">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>#N/A</v>
       </c>
       <c r="C796" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="797" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A797" t="s">
-        <v>296</v>
-      </c>
-      <c r="B797" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_AWS_timestamp_format</v>
+    <row r="797" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B797" t="e">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>#N/A</v>
       </c>
       <c r="C797" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="798" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A798" t="s">
-        <v>297</v>
-      </c>
-      <c r="B798" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_non_COUNTER_file_name_regex</v>
+    <row r="798" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B798" t="e">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>#N/A</v>
       </c>
       <c r="C798" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="799" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A799" t="s">
-        <v>298</v>
-      </c>
-      <c r="B799" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_empty_string_regex</v>
+    <row r="799" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B799" t="e">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>#N/A</v>
       </c>
       <c r="C799" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="800" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A800" t="s">
-        <v>300</v>
-      </c>
-      <c r="B800" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_annual_stats_homepage</v>
+    <row r="800" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B800" t="e">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>#N/A</v>
       </c>
       <c r="C800" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14469,12 +14661,9 @@
       </c>
     </row>
     <row r="801" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A801" t="s">
-        <v>301</v>
-      </c>
-      <c r="B801" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_show_fiscal_year_details</v>
+      <c r="B801" t="e">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>#N/A</v>
       </c>
       <c r="C801" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14483,11 +14672,11 @@
     </row>
     <row r="802" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A802" t="s">
-        <v>302</v>
+        <v>246</v>
       </c>
       <c r="B802" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_show_fiscal_year_details_submitting_RunAnnualStatsMethodsForm</v>
+        <v>create_COUNTERData_workbook_iterdir_list</v>
       </c>
       <c r="C802" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14496,11 +14685,11 @@
     </row>
     <row r="803" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A803" t="s">
-        <v>303</v>
+        <v>247</v>
       </c>
       <c r="B803" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_show_fiscal_year_details_submitting_EditFiscalYearForm</v>
+        <v>COUNTERData_relation</v>
       </c>
       <c r="C803" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14509,11 +14698,11 @@
     </row>
     <row r="804" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A804" t="s">
-        <v>304</v>
+        <v>248</v>
       </c>
       <c r="B804" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_show_fiscal_year_details_submitting_EditAUCTForm</v>
+        <v>download_destination</v>
       </c>
       <c r="C804" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14522,11 +14711,11 @@
     </row>
     <row r="805" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A805" t="s">
-        <v>306</v>
+        <v>249</v>
       </c>
       <c r="B805" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_ingest_usage_homepage</v>
+        <v>path_to_sample_file</v>
       </c>
       <c r="C805" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14535,11 +14724,11 @@
     </row>
     <row r="806" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A806" t="s">
-        <v>307</v>
+        <v>250</v>
       </c>
       <c r="B806" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_upload_COUNTER_data_via_Excel</v>
+        <v>remove_file_from_S3</v>
       </c>
       <c r="C806" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14548,11 +14737,11 @@
     </row>
     <row r="807" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A807" t="s">
-        <v>308</v>
+        <v>251</v>
       </c>
       <c r="B807" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_upload_COUNTER_data_via_SQL_insert</v>
+        <v>non_COUNTER_AUCT_object_before_upload</v>
       </c>
       <c r="C807" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14561,11 +14750,11 @@
     </row>
     <row r="808" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A808" t="s">
-        <v>309</v>
+        <v>252</v>
       </c>
       <c r="B808" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_match_direct_SUSHI_harvest_result</v>
+        <v>non_COUNTER_AUCT_object_after_upload</v>
       </c>
       <c r="C808" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14574,11 +14763,11 @@
     </row>
     <row r="809" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A809" t="s">
-        <v>310</v>
+        <v>253</v>
       </c>
       <c r="B809" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_harvest_SUSHI_statistics</v>
+        <v>non_COUNTER_file_to_download_from_S3</v>
       </c>
       <c r="C809" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14587,11 +14776,11 @@
     </row>
     <row r="810" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A810" t="s">
-        <v>311</v>
+        <v>254</v>
       </c>
       <c r="B810" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_harvest_SUSHI_statistics</v>
+        <v>header_value</v>
       </c>
       <c r="C810" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14600,11 +14789,11 @@
     </row>
     <row r="811" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A811" t="s">
-        <v>312</v>
+        <v>255</v>
       </c>
       <c r="B811" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_upload_non_COUNTER_reports</v>
+        <v>most_recent_month_with_usage</v>
       </c>
       <c r="C811" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14613,11 +14802,11 @@
     </row>
     <row r="812" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A812" t="s">
-        <v>313</v>
+        <v>256</v>
       </c>
       <c r="B812" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_upload_non_COUNTER_reports</v>
+        <v>match_direct_SUSHI_harvest_result</v>
       </c>
       <c r="C812" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14626,11 +14815,11 @@
     </row>
     <row r="813" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A813" t="s">
-        <v>315</v>
+        <v>257</v>
       </c>
       <c r="B813" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>blank_annualUsageCollectionTracking_data_types</v>
+        <v>COUNTER_reports_offered_by_statistics_source</v>
       </c>
       <c r="C813" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14639,11 +14828,11 @@
     </row>
     <row r="814" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A814" t="s">
-        <v>316</v>
+        <v>258</v>
       </c>
       <c r="B814" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_fiscalYears_CSV_file</v>
+        <v>prepare_HTML_page_for_comparison</v>
       </c>
       <c r="C814" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14652,11 +14841,11 @@
     </row>
     <row r="815" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A815" t="s">
-        <v>317</v>
+        <v>260</v>
       </c>
       <c r="B815" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_annualStatistics_CSV_file</v>
+        <v>test_add_annual_statistic_value</v>
       </c>
       <c r="C815" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14665,11 +14854,11 @@
     </row>
     <row r="816" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A816" t="s">
-        <v>318</v>
+        <v>262</v>
       </c>
       <c r="B816" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_vendors_CSV_file</v>
+        <v>AUCT_fixture_for_SUSHI</v>
       </c>
       <c r="C816" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14678,11 +14867,11 @@
     </row>
     <row r="817" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A817" t="s">
-        <v>319</v>
-      </c>
-      <c r="B817" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_vendorNotes_CSV_file</v>
+        <v>263</v>
+      </c>
+      <c r="B817" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>harvest_R5_SUSHI_result</v>
       </c>
       <c r="C817" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14691,11 +14880,11 @@
     </row>
     <row r="818" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A818" t="s">
-        <v>320</v>
+        <v>265</v>
       </c>
       <c r="B818" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_statisticsSources_CSV_file</v>
+        <v>test_collect_annual_usage_statistics</v>
       </c>
       <c r="C818" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14704,11 +14893,11 @@
     </row>
     <row r="819" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A819" t="s">
-        <v>321</v>
+        <v>266</v>
       </c>
       <c r="B819" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_statisticsSourceNotes_CSV_file</v>
+        <v>sample_FileStorage_object</v>
       </c>
       <c r="C819" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14717,11 +14906,11 @@
     </row>
     <row r="820" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A820" t="s">
-        <v>322</v>
+        <v>267</v>
       </c>
       <c r="B820" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_resourceSources_CSV_file</v>
+        <v>test_upload_nonstandard_usage_file</v>
       </c>
       <c r="C820" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14730,11 +14919,11 @@
     </row>
     <row r="821" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A821" t="s">
-        <v>323</v>
+        <v>268</v>
       </c>
       <c r="B821" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_resourceSourceNotes_CSV_file</v>
+        <v>test_download_nonstandard_usage_file</v>
       </c>
       <c r="C821" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14743,11 +14932,11 @@
     </row>
     <row r="822" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A822" t="s">
-        <v>324</v>
+        <v>270</v>
       </c>
       <c r="B822" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_statisticsResourceSources_CSV_file</v>
+        <v>test_flask_app_creation</v>
       </c>
       <c r="C822" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14756,11 +14945,11 @@
     </row>
     <row r="823" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A823" t="s">
-        <v>325</v>
+        <v>271</v>
       </c>
       <c r="B823" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_blank_annualUsageCollectionTracking_CSV_file</v>
+        <v>test_flask_client_creation</v>
       </c>
       <c r="C823" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14769,11 +14958,11 @@
     </row>
     <row r="824" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A824" t="s">
-        <v>326</v>
+        <v>272</v>
       </c>
       <c r="B824" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>create_annualUsageCollectionTracking_CSV_file</v>
+        <v>test_SQLAlchemy_engine_creation</v>
       </c>
       <c r="C824" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14782,11 +14971,11 @@
     </row>
     <row r="825" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A825" t="s">
-        <v>327</v>
+        <v>273</v>
       </c>
       <c r="B825" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_collect_FY_and_vendor_data</v>
+        <v>test_homepage</v>
       </c>
       <c r="C825" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14795,11 +14984,11 @@
     </row>
     <row r="826" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A826" t="s">
-        <v>328</v>
+        <v>274</v>
       </c>
       <c r="B826" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_collect_FY_and_vendor_data</v>
+        <v>test_404_page</v>
       </c>
       <c r="C826" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14808,11 +14997,11 @@
     </row>
     <row r="827" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A827" t="s">
-        <v>329</v>
+        <v>275</v>
       </c>
       <c r="B827" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_collect_sources_data</v>
+        <v>test_load_data_into_database</v>
       </c>
       <c r="C827" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14821,11 +15010,11 @@
     </row>
     <row r="828" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A828" t="s">
-        <v>330</v>
+        <v>276</v>
       </c>
       <c r="B828" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_collect_AUCT_and_historical_COUNTER_data</v>
+        <v>test_query_database</v>
       </c>
       <c r="C828" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14834,11 +15023,11 @@
     </row>
     <row r="829" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A829" t="s">
-        <v>331</v>
+        <v>277</v>
       </c>
       <c r="B829" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_collect_AUCT_and_historical_COUNTER_data</v>
+        <v>test_loading_connected_data_into_other_relation</v>
       </c>
       <c r="C829" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14847,11 +15036,11 @@
     </row>
     <row r="830" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A830" t="s">
-        <v>332</v>
+        <v>278</v>
       </c>
       <c r="B830" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_upload_historical_non_COUNTER_usage</v>
+        <v>test_download_file</v>
       </c>
       <c r="C830" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14860,11 +15049,11 @@
     </row>
     <row r="831" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A831" t="s">
-        <v>333</v>
+        <v>279</v>
       </c>
       <c r="B831" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>"files_for_test_upload_historical_non_COUNTER_usage._files_for_test_upload_historical_non_COUNTER_usage"</v>
+        <v>test_first_new_PK_value</v>
       </c>
       <c r="C831" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14873,11 +15062,11 @@
     </row>
     <row r="832" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A832" t="s">
-        <v>335</v>
+        <v>280</v>
       </c>
       <c r="B832" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_upload_historical_non_COUNTER_usage</v>
+        <v>test_change_single_field_dataframe_into_series</v>
       </c>
       <c r="C832" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14886,11 +15075,11 @@
     </row>
     <row r="833" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A833" t="s">
-        <v>337</v>
+        <v>281</v>
       </c>
       <c r="B833" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_login_homepage</v>
+        <v>test_restore_boolean_values_to_boolean_field</v>
       </c>
       <c r="C833" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14899,11 +15088,11 @@
     </row>
     <row r="834" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A834" t="s">
-        <v>338</v>
+        <v>282</v>
       </c>
       <c r="B834" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_logging_in</v>
+        <v>test_upload_file_to_S3_bucket</v>
       </c>
       <c r="C834" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14912,11 +15101,11 @@
     </row>
     <row r="835" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A835" t="s">
-        <v>339</v>
+        <v>283</v>
       </c>
       <c r="B835" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_logging_in_as_admin</v>
+        <v>test_create_AUCT_SelectField_options</v>
       </c>
       <c r="C835" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14925,11 +15114,11 @@
     </row>
     <row r="836" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A836" t="s">
-        <v>340</v>
+        <v>284</v>
       </c>
       <c r="B836" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_creating_an_account</v>
+        <v>test_truncate_longer_lines</v>
       </c>
       <c r="C836" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14938,11 +15127,11 @@
     </row>
     <row r="837" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A837" t="s">
-        <v>342</v>
+        <v>285</v>
       </c>
       <c r="B837" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_view_lists_homepage</v>
+        <v>vendors_relation_after_test_update_database</v>
       </c>
       <c r="C837" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14951,11 +15140,11 @@
     </row>
     <row r="838" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A838" t="s">
-        <v>343</v>
+        <v>286</v>
       </c>
       <c r="B838" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_view_list_record</v>
+        <v>test_update_database</v>
       </c>
       <c r="C838" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14964,11 +15153,11 @@
     </row>
     <row r="839" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A839" t="s">
-        <v>344</v>
+        <v>287</v>
       </c>
       <c r="B839" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_view_list_record</v>
+        <v>vendors_relation_after_test_update_database_with_insert_statement</v>
       </c>
       <c r="C839" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14977,11 +15166,11 @@
     </row>
     <row r="840" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A840" t="s">
-        <v>345</v>
+        <v>288</v>
       </c>
       <c r="B840" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_edit_list_record_for_existing_record</v>
+        <v>test_update_database_with_insert_statement</v>
       </c>
       <c r="C840" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -14990,11 +15179,11 @@
     </row>
     <row r="841" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A841" t="s">
-        <v>346</v>
+        <v>289</v>
       </c>
       <c r="B841" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_edit_list_record_for_new_record</v>
+        <v>test_prepare_HTML_page_for_comparison</v>
       </c>
       <c r="C841" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15003,11 +15192,11 @@
     </row>
     <row r="842" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A842" t="s">
-        <v>347</v>
+        <v>290</v>
       </c>
       <c r="B842" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_edit_list_record</v>
+        <v>file_name_stem_and_data</v>
       </c>
       <c r="C842" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15016,11 +15205,11 @@
     </row>
     <row r="843" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A843" t="s">
-        <v>349</v>
+        <v>291</v>
       </c>
       <c r="B843" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>COUNTER_download_CSV</v>
+        <v>test_save_unconverted_data_via_upload</v>
       </c>
       <c r="C843" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15029,11 +15218,11 @@
     </row>
     <row r="844" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A844" t="s">
-        <v>350</v>
+        <v>292</v>
       </c>
       <c r="B844" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_COUNTER_fixed_vocab_list</v>
+        <v>test_ISSN_regex</v>
       </c>
       <c r="C844" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15042,11 +15231,11 @@
     </row>
     <row r="845" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A845" t="s">
-        <v>351</v>
+        <v>293</v>
       </c>
       <c r="B845" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_set_encoding</v>
+        <v>test_ISBN_regex</v>
       </c>
       <c r="C845" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15055,11 +15244,11 @@
     </row>
     <row r="846" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A846" t="s">
-        <v>352</v>
+        <v>294</v>
       </c>
       <c r="B846" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_view_usage_homepage</v>
+        <v>test_last_day_of_month</v>
       </c>
       <c r="C846" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15068,11 +15257,11 @@
     </row>
     <row r="847" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A847" t="s">
-        <v>353</v>
+        <v>295</v>
       </c>
       <c r="B847" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_run_custom_SQL_query</v>
+        <v>test_extract_value_from_single_value_df</v>
       </c>
       <c r="C847" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15081,11 +15270,11 @@
     </row>
     <row r="848" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A848" t="s">
-        <v>354</v>
+        <v>296</v>
       </c>
       <c r="B848" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_use_predefined_SQL_query</v>
+        <v>test_AWS_timestamp_format</v>
       </c>
       <c r="C848" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15094,11 +15283,11 @@
     </row>
     <row r="849" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A849" t="s">
-        <v>355</v>
+        <v>297</v>
       </c>
       <c r="B849" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>start_query_wizard_form_data</v>
+        <v>test_non_COUNTER_file_name_regex</v>
       </c>
       <c r="C849" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15107,11 +15296,11 @@
     </row>
     <row r="850" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A850" t="s">
-        <v>356</v>
+        <v>298</v>
       </c>
       <c r="B850" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_start_query_wizard</v>
+        <v>test_empty_string_regex</v>
       </c>
       <c r="C850" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15120,11 +15309,11 @@
     </row>
     <row r="851" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A851" t="s">
-        <v>357</v>
+        <v>300</v>
       </c>
       <c r="B851" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_query_wizard_sort_redirect</v>
+        <v>test_GET_request_for_annual_stats_homepage</v>
       </c>
       <c r="C851" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15133,11 +15322,11 @@
     </row>
     <row r="852" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A852" t="s">
-        <v>358</v>
+        <v>301</v>
       </c>
       <c r="B852" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>PR_parameters</v>
+        <v>test_GET_request_for_show_fiscal_year_details</v>
       </c>
       <c r="C852" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15146,11 +15335,11 @@
     </row>
     <row r="853" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A853" t="s">
-        <v>359</v>
+        <v>302</v>
       </c>
       <c r="B853" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_construct_PR_query_with_wizard</v>
+        <v>test_show_fiscal_year_details_submitting_RunAnnualStatsMethodsForm</v>
       </c>
       <c r="C853" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15159,11 +15348,11 @@
     </row>
     <row r="854" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A854" t="s">
-        <v>360</v>
+        <v>303</v>
       </c>
       <c r="B854" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>DR_parameters</v>
+        <v>test_show_fiscal_year_details_submitting_EditFiscalYearForm</v>
       </c>
       <c r="C854" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15172,11 +15361,11 @@
     </row>
     <row r="855" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A855" t="s">
-        <v>361</v>
+        <v>304</v>
       </c>
       <c r="B855" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_construct_DR_query_with_wizard</v>
+        <v>test_show_fiscal_year_details_submitting_EditAUCTForm</v>
       </c>
       <c r="C855" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15185,11 +15374,11 @@
     </row>
     <row r="856" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A856" t="s">
-        <v>362</v>
+        <v>306</v>
       </c>
       <c r="B856" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>TR_parameters</v>
+        <v>test_ingest_usage_homepage</v>
       </c>
       <c r="C856" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15198,11 +15387,11 @@
     </row>
     <row r="857" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A857" t="s">
-        <v>363</v>
+        <v>307</v>
       </c>
       <c r="B857" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_construct_TR_query_with_wizard</v>
+        <v>test_upload_COUNTER_data_via_Excel</v>
       </c>
       <c r="C857" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15211,11 +15400,11 @@
     </row>
     <row r="858" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A858" t="s">
-        <v>364</v>
+        <v>308</v>
       </c>
       <c r="B858" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>IR_parameters</v>
+        <v>test_upload_COUNTER_data_via_SQL_insert</v>
       </c>
       <c r="C858" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15224,11 +15413,11 @@
     </row>
     <row r="859" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A859" t="s">
-        <v>365</v>
+        <v>309</v>
       </c>
       <c r="B859" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_construct_IR_query_with_wizard</v>
+        <v>test_match_direct_SUSHI_harvest_result</v>
       </c>
       <c r="C859" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15237,11 +15426,11 @@
     </row>
     <row r="860" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A860" t="s">
-        <v>366</v>
+        <v>310</v>
       </c>
       <c r="B860" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>construct_PR_query_with_wizard_without_string_match</v>
+        <v>test_GET_request_for_harvest_SUSHI_statistics</v>
       </c>
       <c r="C860" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15250,11 +15439,11 @@
     </row>
     <row r="861" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A861" t="s">
-        <v>367</v>
+        <v>311</v>
       </c>
       <c r="B861" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_GET_request_for_download_non_COUNTER_usage</v>
+        <v>test_harvest_SUSHI_statistics</v>
       </c>
       <c r="C861" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15263,11 +15452,11 @@
     </row>
     <row r="862" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A862" t="s">
-        <v>368</v>
+        <v>312</v>
       </c>
       <c r="B862" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_download_non_COUNTER_usage</v>
+        <v>test_GET_request_for_upload_non_COUNTER_reports</v>
       </c>
       <c r="C862" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15276,11 +15465,11 @@
     </row>
     <row r="863" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A863" t="s">
-        <v>370</v>
+        <v>313</v>
       </c>
       <c r="B863" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_PR_response_R5_JSON_dict</v>
+        <v>test_upload_non_COUNTER_reports</v>
       </c>
       <c r="C863" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15289,11 +15478,11 @@
     </row>
     <row r="864" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A864" t="s">
-        <v>371</v>
+        <v>315</v>
       </c>
       <c r="B864" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_PR_response_R5_dataframe</v>
+        <v>blank_annualUsageCollectionTracking_data_types</v>
       </c>
       <c r="C864" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15302,11 +15491,11 @@
     </row>
     <row r="865" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A865" t="s">
-        <v>372</v>
+        <v>316</v>
       </c>
       <c r="B865" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_DR_response_R5_JSON_dict</v>
+        <v>create_fiscalYears_CSV_file</v>
       </c>
       <c r="C865" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15315,11 +15504,11 @@
     </row>
     <row r="866" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A866" t="s">
-        <v>373</v>
+        <v>317</v>
       </c>
       <c r="B866" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_DR_response_R5_dataframe</v>
+        <v>create_annualStatistics_CSV_file</v>
       </c>
       <c r="C866" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15328,11 +15517,11 @@
     </row>
     <row r="867" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A867" t="s">
-        <v>374</v>
+        <v>318</v>
       </c>
       <c r="B867" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_TR_response_R5_JSON_dict</v>
+        <v>create_vendors_CSV_file</v>
       </c>
       <c r="C867" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15341,11 +15530,11 @@
     </row>
     <row r="868" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A868" t="s">
-        <v>375</v>
+        <v>319</v>
       </c>
       <c r="B868" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_TR_response_R5_dataframe</v>
+        <v>create_vendorNotes_CSV_file</v>
       </c>
       <c r="C868" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15354,11 +15543,11 @@
     </row>
     <row r="869" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A869" t="s">
-        <v>376</v>
+        <v>320</v>
       </c>
       <c r="B869" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_IR_response_R5_JSON_dict</v>
+        <v>create_statisticsSources_CSV_file</v>
       </c>
       <c r="C869" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15367,11 +15556,11 @@
     </row>
     <row r="870" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A870" t="s">
-        <v>377</v>
+        <v>321</v>
       </c>
       <c r="B870" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_IR_response_R5_dataframe</v>
+        <v>create_statisticsSourceNotes_CSV_file</v>
       </c>
       <c r="C870" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15380,11 +15569,11 @@
     </row>
     <row r="871" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A871" t="s">
-        <v>378</v>
+        <v>322</v>
       </c>
       <c r="B871" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_PR_response_R5b1_JSON_dict</v>
+        <v>create_resourceSources_CSV_file</v>
       </c>
       <c r="C871" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15393,11 +15582,11 @@
     </row>
     <row r="872" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A872" t="s">
-        <v>379</v>
+        <v>323</v>
       </c>
       <c r="B872" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_PR_response_R5b1_dataframe</v>
+        <v>create_resourceSourceNotes_CSV_file</v>
       </c>
       <c r="C872" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15406,11 +15595,11 @@
     </row>
     <row r="873" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A873" t="s">
-        <v>380</v>
+        <v>324</v>
       </c>
       <c r="B873" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_DR_response_R5b1_JSON_dict</v>
+        <v>create_statisticsResourceSources_CSV_file</v>
       </c>
       <c r="C873" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15419,11 +15608,11 @@
     </row>
     <row r="874" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A874" t="s">
-        <v>381</v>
+        <v>325</v>
       </c>
       <c r="B874" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_DR_response_R5b1_dataframe</v>
+        <v>create_blank_annualUsageCollectionTracking_CSV_file</v>
       </c>
       <c r="C874" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15432,11 +15621,11 @@
     </row>
     <row r="875" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A875" t="s">
-        <v>382</v>
+        <v>326</v>
       </c>
       <c r="B875" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_TR_response_R5b1_JSON_dict</v>
+        <v>create_annualUsageCollectionTracking_CSV_file</v>
       </c>
       <c r="C875" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15445,11 +15634,11 @@
     </row>
     <row r="876" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A876" t="s">
-        <v>383</v>
+        <v>327</v>
       </c>
       <c r="B876" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_TR_response_R5b1_dataframe</v>
+        <v>test_GET_request_for_collect_FY_and_vendor_data</v>
       </c>
       <c r="C876" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15458,11 +15647,11 @@
     </row>
     <row r="877" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A877" t="s">
-        <v>384</v>
+        <v>328</v>
       </c>
       <c r="B877" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_IR_response_R5b1_JSON_dict</v>
+        <v>test_collect_FY_and_vendor_data</v>
       </c>
       <c r="C877" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15471,11 +15660,11 @@
     </row>
     <row r="878" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A878" t="s">
-        <v>385</v>
+        <v>329</v>
       </c>
       <c r="B878" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_SUSHI_IR_response_R5b1_dataframe</v>
+        <v>test_collect_sources_data</v>
       </c>
       <c r="C878" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15484,11 +15673,11 @@
     </row>
     <row r="879" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A879" t="s">
-        <v>386</v>
+        <v>330</v>
       </c>
       <c r="B879" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5_PR</v>
+        <v>test_GET_request_for_collect_AUCT_and_historical_COUNTER_data</v>
       </c>
       <c r="C879" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15497,11 +15686,11 @@
     </row>
     <row r="880" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A880" t="s">
-        <v>387</v>
+        <v>331</v>
       </c>
       <c r="B880" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5_DR</v>
+        <v>test_collect_AUCT_and_historical_COUNTER_data</v>
       </c>
       <c r="C880" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15510,11 +15699,11 @@
     </row>
     <row r="881" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A881" t="s">
-        <v>388</v>
+        <v>332</v>
       </c>
       <c r="B881" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5_TR</v>
+        <v>test_GET_request_for_upload_historical_non_COUNTER_usage</v>
       </c>
       <c r="C881" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15523,11 +15712,11 @@
     </row>
     <row r="882" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A882" t="s">
-        <v>389</v>
+        <v>333</v>
       </c>
       <c r="B882" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5_IR</v>
+        <v>"files_for_test_upload_historical_non_COUNTER_usage._files_for_test_upload_historical_non_COUNTER_usage"</v>
       </c>
       <c r="C882" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15536,11 +15725,11 @@
     </row>
     <row r="883" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A883" t="s">
-        <v>390</v>
+        <v>335</v>
       </c>
       <c r="B883" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5b1_PR</v>
+        <v>test_upload_historical_non_COUNTER_usage</v>
       </c>
       <c r="C883" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15549,11 +15738,11 @@
     </row>
     <row r="884" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A884" t="s">
-        <v>391</v>
+        <v>337</v>
       </c>
       <c r="B884" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5b1_DR</v>
+        <v>test_login_homepage</v>
       </c>
       <c r="C884" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15562,11 +15751,11 @@
     </row>
     <row r="885" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A885" t="s">
-        <v>392</v>
+        <v>338</v>
       </c>
       <c r="B885" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5b1_TR</v>
+        <v>test_logging_in</v>
       </c>
       <c r="C885" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15575,11 +15764,11 @@
     </row>
     <row r="886" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A886" t="s">
-        <v>393</v>
+        <v>339</v>
       </c>
       <c r="B886" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_R5b1_IR</v>
+        <v>test_logging_in_as_admin</v>
       </c>
       <c r="C886" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15588,11 +15777,11 @@
     </row>
     <row r="887" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A887" t="s">
-        <v>395</v>
+        <v>340</v>
       </c>
       <c r="B887" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>FY2020_FiscalYears_object</v>
+        <v>test_creating_an_account</v>
       </c>
       <c r="C887" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15601,11 +15790,11 @@
     </row>
     <row r="888" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A888" t="s">
-        <v>396</v>
+        <v>342</v>
       </c>
       <c r="B888" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_depreciated_ACRL_60b</v>
+        <v>test_view_lists_homepage</v>
       </c>
       <c r="C888" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15614,11 +15803,11 @@
     </row>
     <row r="889" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A889" t="s">
-        <v>397</v>
+        <v>343</v>
       </c>
       <c r="B889" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_depreciated_ACRL_63</v>
+        <v>test_GET_request_for_view_list_record</v>
       </c>
       <c r="C889" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15627,11 +15816,11 @@
     </row>
     <row r="890" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A890" t="s">
-        <v>398</v>
+        <v>344</v>
       </c>
       <c r="B890" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_ACRL_61a</v>
+        <v>test_view_list_record</v>
       </c>
       <c r="C890" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15640,11 +15829,11 @@
     </row>
     <row r="891" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A891" t="s">
-        <v>399</v>
+        <v>345</v>
       </c>
       <c r="B891" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_ACRL_61b</v>
+        <v>test_GET_request_for_edit_list_record_for_existing_record</v>
       </c>
       <c r="C891" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15653,11 +15842,11 @@
     </row>
     <row r="892" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A892" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="B892" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_ARL_18</v>
+        <v>test_GET_request_for_edit_list_record_for_new_record</v>
       </c>
       <c r="C892" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15666,11 +15855,11 @@
     </row>
     <row r="893" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A893" t="s">
-        <v>401</v>
+        <v>347</v>
       </c>
       <c r="B893" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_ARL_19</v>
+        <v>test_edit_list_record</v>
       </c>
       <c r="C893" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15679,11 +15868,11 @@
     </row>
     <row r="894" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A894" t="s">
-        <v>402</v>
+        <v>349</v>
       </c>
       <c r="B894" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_calculate_ARL_20</v>
+        <v>COUNTER_download_CSV</v>
       </c>
       <c r="C894" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15692,11 +15881,11 @@
     </row>
     <row r="895" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A895" t="s">
-        <v>403</v>
+        <v>350</v>
       </c>
       <c r="B895" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>FY2023_FiscalYears_object_and_record</v>
+        <v>test_create_COUNTER_fixed_vocab_list</v>
       </c>
       <c r="C895" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15705,11 +15894,11 @@
     </row>
     <row r="896" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A896" t="s">
-        <v>404</v>
+        <v>351</v>
       </c>
       <c r="B896" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>load_new_record_into_fiscalYears</v>
+        <v>test_set_encoding</v>
       </c>
       <c r="C896" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15718,11 +15907,11 @@
     </row>
     <row r="897" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A897" t="s">
-        <v>405</v>
+        <v>352</v>
       </c>
       <c r="B897" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_usage_tracking_records_for_fiscal_year</v>
+        <v>test_view_usage_homepage</v>
       </c>
       <c r="C897" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15731,11 +15920,11 @@
     </row>
     <row r="898" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A898" t="s">
-        <v>406</v>
+        <v>353</v>
       </c>
       <c r="B898" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>FY2022_FiscalYears_object</v>
+        <v>test_run_custom_SQL_query</v>
       </c>
       <c r="C898" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15744,11 +15933,11 @@
     </row>
     <row r="899" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A899" t="s">
-        <v>3</v>
+        <v>354</v>
       </c>
       <c r="B899" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_collect_fiscal_year_usage_statistics</v>
+        <v>test_use_predefined_SQL_query</v>
       </c>
       <c r="C899" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15757,11 +15946,11 @@
     </row>
     <row r="900" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A900" t="s">
-        <v>408</v>
+        <v>355</v>
       </c>
       <c r="B900" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_add_access_stop_date</v>
+        <v>start_query_wizard_form_data</v>
       </c>
       <c r="C900" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15770,11 +15959,11 @@
     </row>
     <row r="901" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A901" t="s">
-        <v>409</v>
+        <v>356</v>
       </c>
       <c r="B901" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_remove_access_stop_date</v>
+        <v>test_start_query_wizard</v>
       </c>
       <c r="C901" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15783,11 +15972,11 @@
     </row>
     <row r="902" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A902" t="s">
-        <v>410</v>
+        <v>357</v>
       </c>
       <c r="B902" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_change_StatisticsSource</v>
+        <v>test_GET_query_wizard_sort_redirect</v>
       </c>
       <c r="C902" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15796,11 +15985,11 @@
     </row>
     <row r="903" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A903" t="s">
-        <v>411</v>
-      </c>
-      <c r="B903" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_add_note</v>
+        <v>358</v>
+      </c>
+      <c r="B903" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>PR_parameters</v>
       </c>
       <c r="C903" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15809,11 +15998,11 @@
     </row>
     <row r="904" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A904" t="s">
-        <v>413</v>
+        <v>359</v>
       </c>
       <c r="B904" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_format_list_for_stdout_with_list</v>
+        <v>test_construct_PR_query_with_wizard</v>
       </c>
       <c r="C904" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15822,11 +16011,11 @@
     </row>
     <row r="905" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A905" t="s">
-        <v>414</v>
+        <v>360</v>
       </c>
       <c r="B905" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_format_list_for_stdout_with_generator</v>
+        <v>DR_parameters</v>
       </c>
       <c r="C905" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15835,11 +16024,11 @@
     </row>
     <row r="906" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A906" t="s">
-        <v>415</v>
+        <v>361</v>
       </c>
       <c r="B906" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_remove_IDE_spacing_from_statement</v>
+        <v>test_construct_DR_query_with_wizard</v>
       </c>
       <c r="C906" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15848,11 +16037,11 @@
     </row>
     <row r="907" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A907" t="s">
-        <v>417</v>
+        <v>362</v>
       </c>
       <c r="B907" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>current_month_like_most_recent_month_with_usage</v>
+        <v>TR_parameters</v>
       </c>
       <c r="C907" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15861,11 +16050,11 @@
     </row>
     <row r="908" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A908" t="s">
-        <v>4</v>
+        <v>363</v>
       </c>
       <c r="B908" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>StatisticsSources_fixture</v>
+        <v>test_construct_TR_query_with_wizard</v>
       </c>
       <c r="C908" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15874,11 +16063,11 @@
     </row>
     <row r="909" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A909" t="s">
-        <v>418</v>
+        <v>364</v>
       </c>
       <c r="B909" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_fetch_SUSHI_information_for_API</v>
+        <v>IR_parameters</v>
       </c>
       <c r="C909" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15887,11 +16076,11 @@
     </row>
     <row r="910" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A910" t="s">
-        <v>419</v>
+        <v>365</v>
       </c>
       <c r="B910" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_fetch_SUSHI_information_for_display</v>
+        <v>test_construct_IR_query_with_wizard</v>
       </c>
       <c r="C910" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15900,11 +16089,11 @@
     </row>
     <row r="911" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A911" t="s">
-        <v>420</v>
-      </c>
-      <c r="B911" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>SUSHI_credentials_fixture</v>
+        <v>366</v>
+      </c>
+      <c r="B911" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>construct_PR_query_with_wizard_without_string_match</v>
       </c>
       <c r="C911" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15913,11 +16102,11 @@
     </row>
     <row r="912" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A912" t="s">
-        <v>421</v>
+        <v>367</v>
       </c>
       <c r="B912" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>reports_offered_by_StatisticsSource_fixture</v>
+        <v>test_GET_request_for_download_non_COUNTER_usage</v>
       </c>
       <c r="C912" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15926,11 +16115,11 @@
     </row>
     <row r="913" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A913" t="s">
-        <v>422</v>
+        <v>368</v>
       </c>
       <c r="B913" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_COUNTER_reports_offered_by_statistics_source</v>
+        <v>test_download_non_COUNTER_usage</v>
       </c>
       <c r="C913" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15939,11 +16128,11 @@
     </row>
     <row r="914" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A914" t="s">
-        <v>423</v>
+        <v>370</v>
       </c>
       <c r="B914" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_check_if_data_in_database_no</v>
+        <v>sample_SUSHI_PR_response_R5_JSON_dict</v>
       </c>
       <c r="C914" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15952,11 +16141,11 @@
     </row>
     <row r="915" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A915" t="s">
-        <v>424</v>
+        <v>371</v>
       </c>
       <c r="B915" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_check_if_data_in_database_yes</v>
+        <v>sample_SUSHI_PR_response_R5_dataframe</v>
       </c>
       <c r="C915" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15965,11 +16154,11 @@
     </row>
     <row r="916" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A916" t="s">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="B916" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_harvest_single_report</v>
+        <v>sample_SUSHI_DR_response_R5_JSON_dict</v>
       </c>
       <c r="C916" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15978,11 +16167,11 @@
     </row>
     <row r="917" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A917" t="s">
-        <v>426</v>
+        <v>373</v>
       </c>
       <c r="B917" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_harvest_single_report_with_partial_date_range</v>
+        <v>sample_SUSHI_DR_response_R5_dataframe</v>
       </c>
       <c r="C917" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -15991,11 +16180,11 @@
     </row>
     <row r="918" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A918" t="s">
-        <v>427</v>
+        <v>374</v>
       </c>
       <c r="B918" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_harvest_R5_SUSHI</v>
+        <v>sample_SUSHI_TR_response_R5_JSON_dict</v>
       </c>
       <c r="C918" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16004,11 +16193,11 @@
     </row>
     <row r="919" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A919" t="s">
-        <v>428</v>
+        <v>375</v>
       </c>
       <c r="B919" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_harvest_R5_SUSHI_with_report_to_harvest</v>
+        <v>sample_SUSHI_TR_response_R5_dataframe</v>
       </c>
       <c r="C919" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16017,11 +16206,11 @@
     </row>
     <row r="920" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A920" t="s">
-        <v>429</v>
+        <v>376</v>
       </c>
       <c r="B920" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_harvest_R5_SUSHI_with_invalid_dates</v>
+        <v>sample_SUSHI_IR_response_R5_JSON_dict</v>
       </c>
       <c r="C920" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16030,11 +16219,11 @@
     </row>
     <row r="921" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A921" t="s">
-        <v>430</v>
+        <v>377</v>
       </c>
       <c r="B921" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>month_before_month_like_most_recent_month_with_usage</v>
+        <v>sample_SUSHI_IR_response_R5_dataframe</v>
       </c>
       <c r="C921" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16043,11 +16232,11 @@
     </row>
     <row r="922" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A922" t="s">
-        <v>431</v>
-      </c>
-      <c r="B922" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>harvest_R5_SUSHI_result</v>
+        <v>378</v>
+      </c>
+      <c r="B922" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>sample_SUSHI_PR_response_R5b1_JSON_dict</v>
       </c>
       <c r="C922" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16056,11 +16245,11 @@
     </row>
     <row r="923" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A923" t="s">
-        <v>432</v>
+        <v>379</v>
       </c>
       <c r="B923" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_collect_usage_statistics</v>
+        <v>sample_SUSHI_PR_response_R5b1_dataframe</v>
       </c>
       <c r="C923" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16069,11 +16258,11 @@
     </row>
     <row r="924" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A924" t="s">
-        <v>433</v>
-      </c>
-      <c r="B924" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_add_note</v>
+        <v>380</v>
+      </c>
+      <c r="B924" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>sample_SUSHI_DR_response_R5b1_JSON_dict</v>
       </c>
       <c r="C924" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16082,11 +16271,11 @@
     </row>
     <row r="925" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A925" t="s">
-        <v>434</v>
+        <v>381</v>
       </c>
       <c r="B925" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>partially_duplicate_COUNTER_data</v>
+        <v>sample_SUSHI_DR_response_R5b1_dataframe</v>
       </c>
       <c r="C925" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16095,11 +16284,11 @@
     </row>
     <row r="926" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A926" t="s">
-        <v>435</v>
+        <v>382</v>
       </c>
       <c r="B926" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>non_duplicate_COUNTER_data</v>
+        <v>sample_SUSHI_TR_response_R5b1_JSON_dict</v>
       </c>
       <c r="C926" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16108,11 +16297,11 @@
     </row>
     <row r="927" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A927" t="s">
-        <v>436</v>
+        <v>383</v>
       </c>
       <c r="B927" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_check_if_data_already_in_COUNTERData</v>
+        <v>sample_SUSHI_TR_response_R5b1_dataframe</v>
       </c>
       <c r="C927" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16121,11 +16310,11 @@
     </row>
     <row r="928" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A928" t="s">
-        <v>438</v>
-      </c>
-      <c r="B928" s="2" t="str">
-        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>SUSHI_credentials_fixture</v>
+        <v>384</v>
+      </c>
+      <c r="B928" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>sample_SUSHI_IR_response_R5b1_JSON_dict</v>
       </c>
       <c r="C928" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16134,11 +16323,11 @@
     </row>
     <row r="929" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A929" t="s">
-        <v>440</v>
+        <v>385</v>
       </c>
       <c r="B929" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>StatisticsSource_instance_name</v>
+        <v>sample_SUSHI_IR_response_R5b1_dataframe</v>
       </c>
       <c r="C929" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16147,11 +16336,11 @@
     </row>
     <row r="930" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A930" t="s">
-        <v>441</v>
+        <v>386</v>
       </c>
       <c r="B930" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_status_call</v>
+        <v>test_create_dataframe_from_R5_PR</v>
       </c>
       <c r="C930" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16160,11 +16349,11 @@
     </row>
     <row r="931" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A931" t="s">
-        <v>442</v>
+        <v>387</v>
       </c>
       <c r="B931" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_status_call_validity</v>
+        <v>test_create_dataframe_from_R5_DR</v>
       </c>
       <c r="C931" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16173,11 +16362,11 @@
     </row>
     <row r="932" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A932" t="s">
-        <v>443</v>
+        <v>388</v>
       </c>
       <c r="B932" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_reports_call</v>
+        <v>test_create_dataframe_from_R5_TR</v>
       </c>
       <c r="C932" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16186,11 +16375,11 @@
     </row>
     <row r="933" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A933" t="s">
-        <v>444</v>
+        <v>389</v>
       </c>
       <c r="B933" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_reports_call_validity</v>
+        <v>test_create_dataframe_from_R5_IR</v>
       </c>
       <c r="C933" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16199,11 +16388,11 @@
     </row>
     <row r="934" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A934" t="s">
-        <v>445</v>
+        <v>390</v>
       </c>
       <c r="B934" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>list_of_reports</v>
+        <v>test_create_dataframe_from_R5b1_PR</v>
       </c>
       <c r="C934" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16212,11 +16401,11 @@
     </row>
     <row r="935" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A935" t="s">
-        <v>446</v>
+        <v>391</v>
       </c>
       <c r="B935" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_PR_call_validity</v>
+        <v>test_create_dataframe_from_R5b1_DR</v>
       </c>
       <c r="C935" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16225,11 +16414,11 @@
     </row>
     <row r="936" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A936" t="s">
-        <v>447</v>
+        <v>392</v>
       </c>
       <c r="B936" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_DR_call_validity</v>
+        <v>test_create_dataframe_from_R5b1_TR</v>
       </c>
       <c r="C936" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16238,11 +16427,11 @@
     </row>
     <row r="937" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A937" t="s">
-        <v>448</v>
+        <v>393</v>
       </c>
       <c r="B937" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_TR_call_validity</v>
+        <v>test_create_dataframe_from_R5b1_IR</v>
       </c>
       <c r="C937" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16251,11 +16440,11 @@
     </row>
     <row r="938" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A938" t="s">
-        <v>449</v>
+        <v>395</v>
       </c>
       <c r="B938" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_IR_call_validity</v>
+        <v>FY2020_FiscalYears_object</v>
       </c>
       <c r="C938" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16264,11 +16453,11 @@
     </row>
     <row r="939" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A939" t="s">
-        <v>450</v>
+        <v>396</v>
       </c>
       <c r="B939" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_call_with_invalid_credentials</v>
+        <v>test_calculate_depreciated_ACRL_60b</v>
       </c>
       <c r="C939" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16277,11 +16466,11 @@
     </row>
     <row r="940" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A940" t="s">
-        <v>452</v>
+        <v>397</v>
       </c>
       <c r="B940" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_COUNTER_report_workbook</v>
+        <v>test_calculate_depreciated_ACRL_63</v>
       </c>
       <c r="C940" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16290,11 +16479,11 @@
     </row>
     <row r="941" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A941" t="s">
-        <v>453</v>
+        <v>398</v>
       </c>
       <c r="B941" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe_from_single_workbook</v>
+        <v>test_calculate_ACRL_61a</v>
       </c>
       <c r="C941" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16303,11 +16492,11 @@
     </row>
     <row r="942" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A942" t="s">
-        <v>454</v>
+        <v>399</v>
       </c>
       <c r="B942" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>sample_COUNTER_report_workbooks</v>
+        <v>test_calculate_ACRL_61b</v>
       </c>
       <c r="C942" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16316,11 +16505,11 @@
     </row>
     <row r="943" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A943" t="s">
-        <v>455</v>
+        <v>400</v>
       </c>
       <c r="B943" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_create_dataframe</v>
+        <v>test_calculate_ARL_18</v>
       </c>
       <c r="C943" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16329,11 +16518,11 @@
     </row>
     <row r="944" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A944" t="s">
-        <v>457</v>
+        <v>401</v>
       </c>
       <c r="B944" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_get_statisticsSources_records</v>
+        <v>test_calculate_ARL_19</v>
       </c>
       <c r="C944" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16342,11 +16531,11 @@
     </row>
     <row r="945" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A945" t="s">
-        <v>458</v>
+        <v>402</v>
       </c>
       <c r="B945" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
-        <v>test_get_resourceSources_records</v>
+        <v>test_calculate_ARL_20</v>
       </c>
       <c r="C945" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
@@ -16355,19 +16544,682 @@
     </row>
     <row r="946" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A946" t="s">
+        <v>403</v>
+      </c>
+      <c r="B946" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>FY2023_FiscalYears_object_and_record</v>
+      </c>
+      <c r="C946" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="947" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A947" t="s">
+        <v>404</v>
+      </c>
+      <c r="B947" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>load_new_record_into_fiscalYears</v>
+      </c>
+      <c r="C947" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="948" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A948" t="s">
+        <v>405</v>
+      </c>
+      <c r="B948" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_create_usage_tracking_records_for_fiscal_year</v>
+      </c>
+      <c r="C948" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="949" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A949" t="s">
+        <v>406</v>
+      </c>
+      <c r="B949" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>FY2022_FiscalYears_object</v>
+      </c>
+      <c r="C949" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="950" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A950" t="s">
+        <v>3</v>
+      </c>
+      <c r="B950" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_collect_fiscal_year_usage_statistics</v>
+      </c>
+      <c r="C950" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="951" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A951" t="s">
+        <v>408</v>
+      </c>
+      <c r="B951" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_add_access_stop_date</v>
+      </c>
+      <c r="C951" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="952" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A952" t="s">
+        <v>409</v>
+      </c>
+      <c r="B952" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_remove_access_stop_date</v>
+      </c>
+      <c r="C952" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="953" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A953" t="s">
+        <v>410</v>
+      </c>
+      <c r="B953" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_change_StatisticsSource</v>
+      </c>
+      <c r="C953" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="954" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A954" t="s">
+        <v>411</v>
+      </c>
+      <c r="B954" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_add_note</v>
+      </c>
+      <c r="C954" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="955" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A955" t="s">
+        <v>413</v>
+      </c>
+      <c r="B955" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_format_list_for_stdout_with_list</v>
+      </c>
+      <c r="C955" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="956" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A956" t="s">
+        <v>414</v>
+      </c>
+      <c r="B956" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_format_list_for_stdout_with_generator</v>
+      </c>
+      <c r="C956" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="957" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A957" t="s">
+        <v>415</v>
+      </c>
+      <c r="B957" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_remove_IDE_spacing_from_statement</v>
+      </c>
+      <c r="C957" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="958" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A958" t="s">
+        <v>417</v>
+      </c>
+      <c r="B958" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>current_month_like_most_recent_month_with_usage</v>
+      </c>
+      <c r="C958" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="959" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A959" t="s">
+        <v>4</v>
+      </c>
+      <c r="B959" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>StatisticsSources_fixture</v>
+      </c>
+      <c r="C959" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="960" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A960" t="s">
+        <v>418</v>
+      </c>
+      <c r="B960" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_fetch_SUSHI_information_for_API</v>
+      </c>
+      <c r="C960" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="961" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A961" t="s">
+        <v>419</v>
+      </c>
+      <c r="B961" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_fetch_SUSHI_information_for_display</v>
+      </c>
+      <c r="C961" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="962" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A962" t="s">
+        <v>420</v>
+      </c>
+      <c r="B962" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>SUSHI_credentials_fixture</v>
+      </c>
+      <c r="C962" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="963" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A963" t="s">
+        <v>421</v>
+      </c>
+      <c r="B963" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>reports_offered_by_StatisticsSource_fixture</v>
+      </c>
+      <c r="C963" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="964" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A964" t="s">
+        <v>422</v>
+      </c>
+      <c r="B964" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_COUNTER_reports_offered_by_statistics_source</v>
+      </c>
+      <c r="C964" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="965" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A965" t="s">
+        <v>423</v>
+      </c>
+      <c r="B965" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_check_if_data_in_database_no</v>
+      </c>
+      <c r="C965" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="966" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A966" t="s">
+        <v>424</v>
+      </c>
+      <c r="B966" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_check_if_data_in_database_yes</v>
+      </c>
+      <c r="C966" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="967" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A967" t="s">
+        <v>425</v>
+      </c>
+      <c r="B967" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_harvest_single_report</v>
+      </c>
+      <c r="C967" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="968" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A968" t="s">
+        <v>426</v>
+      </c>
+      <c r="B968" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_harvest_single_report_with_partial_date_range</v>
+      </c>
+      <c r="C968" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="969" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A969" t="s">
+        <v>427</v>
+      </c>
+      <c r="B969" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_harvest_R5_SUSHI</v>
+      </c>
+      <c r="C969" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="970" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A970" t="s">
+        <v>428</v>
+      </c>
+      <c r="B970" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_harvest_R5_SUSHI_with_report_to_harvest</v>
+      </c>
+      <c r="C970" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="971" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A971" t="s">
+        <v>429</v>
+      </c>
+      <c r="B971" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_harvest_R5_SUSHI_with_invalid_dates</v>
+      </c>
+      <c r="C971" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="972" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A972" t="s">
+        <v>430</v>
+      </c>
+      <c r="B972" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>month_before_month_like_most_recent_month_with_usage</v>
+      </c>
+      <c r="C972" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="973" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A973" t="s">
+        <v>431</v>
+      </c>
+      <c r="B973" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>harvest_R5_SUSHI_result</v>
+      </c>
+      <c r="C973" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="974" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A974" t="s">
+        <v>432</v>
+      </c>
+      <c r="B974" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_collect_usage_statistics</v>
+      </c>
+      <c r="C974" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="975" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A975" t="s">
+        <v>433</v>
+      </c>
+      <c r="B975" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_add_note</v>
+      </c>
+      <c r="C975" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="976" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A976" t="s">
+        <v>434</v>
+      </c>
+      <c r="B976" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>partially_duplicate_COUNTER_data</v>
+      </c>
+      <c r="C976" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="977" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A977" t="s">
+        <v>435</v>
+      </c>
+      <c r="B977" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>non_duplicate_COUNTER_data</v>
+      </c>
+      <c r="C977" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="978" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A978" t="s">
+        <v>436</v>
+      </c>
+      <c r="B978" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_check_if_data_already_in_COUNTERData</v>
+      </c>
+      <c r="C978" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="979" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A979" t="s">
+        <v>438</v>
+      </c>
+      <c r="B979" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>SUSHI_credentials_fixture</v>
+      </c>
+      <c r="C979" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="980" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A980" t="s">
+        <v>440</v>
+      </c>
+      <c r="B980" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>StatisticsSource_instance_name</v>
+      </c>
+      <c r="C980" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="981" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A981" t="s">
+        <v>441</v>
+      </c>
+      <c r="B981" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_status_call</v>
+      </c>
+      <c r="C981" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="982" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A982" t="s">
+        <v>442</v>
+      </c>
+      <c r="B982" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_status_call_validity</v>
+      </c>
+      <c r="C982" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="983" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A983" t="s">
+        <v>443</v>
+      </c>
+      <c r="B983" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_reports_call</v>
+      </c>
+      <c r="C983" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="984" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A984" t="s">
+        <v>444</v>
+      </c>
+      <c r="B984" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_reports_call_validity</v>
+      </c>
+      <c r="C984" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="985" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A985" t="s">
+        <v>445</v>
+      </c>
+      <c r="B985" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>list_of_reports</v>
+      </c>
+      <c r="C985" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="986" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A986" t="s">
+        <v>446</v>
+      </c>
+      <c r="B986" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_PR_call_validity</v>
+      </c>
+      <c r="C986" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="987" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A987" t="s">
+        <v>447</v>
+      </c>
+      <c r="B987" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_DR_call_validity</v>
+      </c>
+      <c r="C987" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="988" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A988" t="s">
+        <v>448</v>
+      </c>
+      <c r="B988" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_TR_call_validity</v>
+      </c>
+      <c r="C988" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="989" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A989" t="s">
+        <v>449</v>
+      </c>
+      <c r="B989" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_IR_call_validity</v>
+      </c>
+      <c r="C989" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="990" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A990" t="s">
+        <v>450</v>
+      </c>
+      <c r="B990" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_call_with_invalid_credentials</v>
+      </c>
+      <c r="C990" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="991" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A991" t="s">
+        <v>452</v>
+      </c>
+      <c r="B991" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>sample_COUNTER_report_workbook</v>
+      </c>
+      <c r="C991" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="992" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A992" t="s">
+        <v>453</v>
+      </c>
+      <c r="B992" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_create_dataframe_from_single_workbook</v>
+      </c>
+      <c r="C992" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="993" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A993" t="s">
+        <v>454</v>
+      </c>
+      <c r="B993" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>sample_COUNTER_report_workbooks</v>
+      </c>
+      <c r="C993" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="994" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A994" t="s">
+        <v>455</v>
+      </c>
+      <c r="B994" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_create_dataframe</v>
+      </c>
+      <c r="C994" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="995" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A995" t="s">
+        <v>457</v>
+      </c>
+      <c r="B995" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_get_statisticsSources_records</v>
+      </c>
+      <c r="C995" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="996" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A996" t="s">
+        <v>458</v>
+      </c>
+      <c r="B996" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
+        <v>test_get_resourceSources_records</v>
+      </c>
+      <c r="C996" t="b">
+        <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="997" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A997" t="s">
         <v>459</v>
       </c>
-      <c r="B946" s="2" t="str">
+      <c r="B997" s="2" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Called Node Name]],Table2[[Node Name]:[Function Name]],2,0)</f>
         <v>test_add_note</v>
       </c>
-      <c r="C946" t="b">
+      <c r="C997" t="b">
         <f>ISERROR(IF(OR(Table3[[#This Row],[Calling Node]]="NULL",ISBLANK(Table3[[#This Row],[Calling Node]])),TRUE,VLOOKUP(Table3[[#This Row],[Calling Node]],Table3[Called Node Name],1,0)))</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C946">
+  <conditionalFormatting sqref="C2:C997">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>